<commit_message>
Added auto complete function and colour eye dropper
</commit_message>
<xml_diff>
--- a/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
+++ b/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
@@ -20,7 +20,7 @@
     <numFmt numFmtId="165" formatCode="[hh]:mm:ss"/>
     <numFmt numFmtId="166" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -64,6 +64,9 @@
       <color rgb="FFFFFFFF"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -220,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -292,13 +295,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -801,11 +807,15 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B6" s="27" t="n"/>
+      <c r="B6" s="27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
       <c r="C6" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-0</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D6" s="29" t="n">
@@ -818,7 +828,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B7" s="27" t="n"/>
+      <c r="B7" s="30" t="n"/>
       <c r="C7" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Why Be Humble?”: 
@@ -835,8 +845,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B8" s="27" t="n"/>
-      <c r="C8" s="30" t="inlineStr">
+      <c r="B8" s="30" t="n"/>
+      <c r="C8" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  2Ki 23:24, 25 —What encouragement does Josiah’s example provide for those who have endured a difficult childhood? (w01 4/15 26 ¶3-4)
 </t>
@@ -852,7 +862,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B9" s="27" t="n"/>
+      <c r="B9" s="30" t="n"/>
       <c r="C9" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 23:16-25 (th study 2)
@@ -872,7 +882,7 @@
     <row r="11">
       <c r="A11" s="15" t="n"/>
       <c r="B11" s="15" t="n"/>
-      <c r="C11" s="31" t="inlineStr">
+      <c r="C11" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -885,8 +895,8 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B12" s="27" t="n"/>
-      <c r="C12" s="30" t="inlineStr">
+      <c r="B12" s="30" t="n"/>
+      <c r="C12" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call Video:  Discussion. Play the video Initial Call: Prayer —Ps 65:2. Stop the video at each pause, and ask the audience the questions that appear in the video.
 </t>
@@ -897,50 +907,50 @@
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="32" t="inlineStr">
+      <c r="A13" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B13" s="15" t="n"/>
-      <c r="C13" s="33" t="inlineStr">
+      <c r="C13" s="34" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Use the sample conversation topic. (th study 1)
 </t>
         </is>
       </c>
-      <c r="D13" s="34" t="n">
+      <c r="D13" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="27" t="n"/>
-      <c r="B14" s="35" t="n"/>
-      <c r="C14" s="27" t="n"/>
-      <c r="D14" s="36" t="n"/>
+      <c r="A14" s="30" t="n"/>
+      <c r="B14" s="36" t="n"/>
+      <c r="C14" s="30" t="n"/>
+      <c r="D14" s="37" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="32" t="inlineStr">
+      <c r="A15" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B15" s="15" t="n"/>
-      <c r="C15" s="37" t="inlineStr">
+      <c r="C15" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 16)
 </t>
         </is>
       </c>
-      <c r="D15" s="34" t="n">
+      <c r="D15" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="27" t="n"/>
-      <c r="B16" s="35" t="n"/>
-      <c r="C16" s="27" t="n"/>
-      <c r="D16" s="36" t="n"/>
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="36" t="n"/>
+      <c r="C16" s="30" t="n"/>
+      <c r="D16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="15" t="n"/>
@@ -955,7 +965,7 @@
         </is>
       </c>
       <c r="B18" s="15" t="n"/>
-      <c r="C18" s="38" t="inlineStr">
+      <c r="C18" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -968,8 +978,8 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B19" s="27" t="n"/>
-      <c r="C19" s="30" t="inlineStr">
+      <c r="B19" s="30" t="n"/>
+      <c r="C19" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Humble or Haughty? (Jas 4:6):  Discussion. Play the video. Then ask the audience: What is the difference between humility and haughtiness? What can we learn from Moses’ example? Why are you determined to remain humble?
 </t>
@@ -985,7 +995,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B20" s="27" t="n"/>
+      <c r="B20" s="30" t="n"/>
       <c r="C20" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 33
@@ -1002,11 +1012,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B21" s="27" t="n"/>
+      <c r="B21" s="30" t="n"/>
       <c r="C21" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-1</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D21" s="29" t="n">
@@ -1097,11 +1107,11 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B28" s="27" t="n"/>
+      <c r="B28" s="30" t="n"/>
       <c r="C28" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-2</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D28" s="29" t="n">
@@ -1114,7 +1124,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B29" s="27" t="n"/>
+      <c r="B29" s="30" t="n"/>
       <c r="C29" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Maintain Your Sense of Urgency”: 
@@ -1131,8 +1141,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B30" s="27" t="n"/>
-      <c r="C30" s="30" t="inlineStr">
+      <c r="B30" s="30" t="n"/>
+      <c r="C30" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  2Ki 24:3, 4 —What do these verses teach us about Jehovah? (w05 8/1 12 ¶1)
 </t>
@@ -1148,7 +1158,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B31" s="27" t="n"/>
+      <c r="B31" s="30" t="n"/>
       <c r="C31" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 24:1-17 (th study 11)
@@ -1168,7 +1178,7 @@
     <row r="33">
       <c r="A33" s="15" t="n"/>
       <c r="B33" s="15" t="n"/>
-      <c r="C33" s="31" t="inlineStr">
+      <c r="C33" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -1181,8 +1191,8 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B34" s="27" t="n"/>
-      <c r="C34" s="30" t="inlineStr">
+      <c r="B34" s="30" t="n"/>
+      <c r="C34" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit Video:  Discussion. Play the video Return Visit: Prayer —1Jo 5:14. Stop the video at each pause, and ask the audience the questions that appear in the video.
 </t>
@@ -1193,50 +1203,50 @@
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="32" t="inlineStr">
+      <c r="A35" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B35" s="15" t="n"/>
-      <c r="C35" s="33" t="inlineStr">
+      <c r="C35" s="34" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Use the sample conversation topic. (th study 15)
 </t>
         </is>
       </c>
-      <c r="D35" s="34" t="n">
+      <c r="D35" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="27" t="n"/>
-      <c r="B36" s="35" t="n"/>
-      <c r="C36" s="27" t="n"/>
-      <c r="D36" s="36" t="n"/>
+      <c r="A36" s="30" t="n"/>
+      <c r="B36" s="36" t="n"/>
+      <c r="C36" s="30" t="n"/>
+      <c r="D36" s="37" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="32" t="inlineStr">
+      <c r="A37" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B37" s="15" t="n"/>
-      <c r="C37" s="37" t="inlineStr">
+      <c r="C37" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 19)
 </t>
         </is>
       </c>
-      <c r="D37" s="34" t="n">
+      <c r="D37" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="27" t="n"/>
-      <c r="B38" s="35" t="n"/>
-      <c r="C38" s="27" t="n"/>
-      <c r="D38" s="36" t="n"/>
+      <c r="A38" s="30" t="n"/>
+      <c r="B38" s="36" t="n"/>
+      <c r="C38" s="30" t="n"/>
+      <c r="D38" s="37" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="15" t="n"/>
@@ -1251,7 +1261,7 @@
         </is>
       </c>
       <c r="B40" s="15" t="n"/>
-      <c r="C40" s="38" t="inlineStr">
+      <c r="C40" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -1264,7 +1274,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B41" s="27" t="n"/>
+      <c r="B41" s="30" t="n"/>
       <c r="C41" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
@@ -1281,7 +1291,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B42" s="27" t="n"/>
+      <c r="B42" s="30" t="n"/>
       <c r="C42" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff section 2 review
@@ -1298,11 +1308,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B43" s="27" t="n"/>
+      <c r="B43" s="30" t="n"/>
       <c r="C43" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-3</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D43" s="29" t="n">
@@ -1393,11 +1403,11 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B50" s="27" t="n"/>
+      <c r="B50" s="30" t="n"/>
       <c r="C50" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-4</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D50" s="29" t="n">
@@ -1410,7 +1420,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B51" s="27" t="n"/>
+      <c r="B51" s="30" t="n"/>
       <c r="C51" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“The Bible —A Book of Fact, Not Fiction”: 
@@ -1427,8 +1437,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B52" s="27" t="n"/>
-      <c r="C52" s="30" t="inlineStr">
+      <c r="B52" s="30" t="n"/>
+      <c r="C52" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 3:1-3 —Why were women occasionally named in genealogical registers? (it-1 911 ¶3-4)
 </t>
@@ -1444,7 +1454,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B53" s="27" t="n"/>
+      <c r="B53" s="30" t="n"/>
       <c r="C53" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 1:43-54 (th study 5)
@@ -1464,7 +1474,7 @@
     <row r="55">
       <c r="A55" s="15" t="n"/>
       <c r="B55" s="15" t="n"/>
-      <c r="C55" s="31" t="inlineStr">
+      <c r="C55" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -1472,73 +1482,73 @@
       <c r="D55" s="25" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="32" t="inlineStr">
+      <c r="A56" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B56" s="15" t="n"/>
-      <c r="C56" s="37" t="inlineStr">
+      <c r="C56" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a magazine to address a topic raised by the householder. (th study 4)
 </t>
         </is>
       </c>
-      <c r="D56" s="34" t="n">
+      <c r="D56" s="35" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="27" t="n"/>
-      <c r="B57" s="35" t="n"/>
-      <c r="C57" s="27" t="n"/>
-      <c r="D57" s="36" t="n"/>
+      <c r="A57" s="30" t="n"/>
+      <c r="B57" s="36" t="n"/>
+      <c r="C57" s="30" t="n"/>
+      <c r="D57" s="37" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="32" t="inlineStr">
+      <c r="A58" s="33" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B58" s="15" t="n"/>
-      <c r="C58" s="37" t="inlineStr">
+      <c r="C58" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 1)
 </t>
         </is>
       </c>
-      <c r="D58" s="34" t="n">
+      <c r="D58" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="27" t="n"/>
-      <c r="B59" s="35" t="n"/>
-      <c r="C59" s="27" t="n"/>
-      <c r="D59" s="36" t="n"/>
+      <c r="A59" s="30" t="n"/>
+      <c r="B59" s="36" t="n"/>
+      <c r="C59" s="30" t="n"/>
+      <c r="D59" s="37" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="32" t="inlineStr">
+      <c r="A60" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B60" s="15" t="n"/>
-      <c r="C60" s="33" t="inlineStr">
+      <c r="C60" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 point 7 and Some People Say (th study 8)
 </t>
         </is>
       </c>
-      <c r="D60" s="34" t="n">
+      <c r="D60" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="27" t="n"/>
-      <c r="B61" s="35" t="n"/>
-      <c r="C61" s="27" t="n"/>
-      <c r="D61" s="36" t="n"/>
+      <c r="A61" s="30" t="n"/>
+      <c r="B61" s="36" t="n"/>
+      <c r="C61" s="30" t="n"/>
+      <c r="D61" s="37" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="15" t="n"/>
@@ -1553,7 +1563,7 @@
         </is>
       </c>
       <c r="B63" s="15" t="n"/>
-      <c r="C63" s="38" t="inlineStr">
+      <c r="C63" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -1566,7 +1576,7 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B64" s="27" t="n"/>
+      <c r="B64" s="30" t="n"/>
       <c r="C64" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Faith in God’s Word”:  Discussion and video.
@@ -1583,7 +1593,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B65" s="27" t="n"/>
+      <c r="B65" s="30" t="n"/>
       <c r="C65" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 34
@@ -1600,11 +1610,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B66" s="27" t="n"/>
+      <c r="B66" s="30" t="n"/>
       <c r="C66" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-5</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D66" s="29" t="n">
@@ -1695,11 +1705,11 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B73" s="27" t="n"/>
+      <c r="B73" s="30" t="n"/>
       <c r="C73" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-6</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D73" s="29" t="n">
@@ -1712,7 +1722,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B74" s="27" t="n"/>
+      <c r="B74" s="30" t="n"/>
       <c r="C74" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“What Do My Prayers Reveal About Me?”: 
@@ -1729,8 +1739,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B75" s="27" t="n"/>
-      <c r="C75" s="30" t="inlineStr">
+      <c r="B75" s="30" t="n"/>
+      <c r="C75" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 5:10 —How can the victory over the Hagrites encourage us when we face seemingly insurmountable obstacles? (w05 10/1 9 ¶7)
 </t>
@@ -1746,7 +1756,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B76" s="27" t="n"/>
+      <c r="B76" s="30" t="n"/>
       <c r="C76" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 6:61-81 (th study 2)
@@ -1766,7 +1776,7 @@
     <row r="78">
       <c r="A78" s="15" t="n"/>
       <c r="B78" s="15" t="n"/>
-      <c r="C78" s="31" t="inlineStr">
+      <c r="C78" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -1774,73 +1784,73 @@
       <c r="D78" s="25" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" s="32" t="inlineStr">
+      <c r="A79" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B79" s="15" t="n"/>
-      <c r="C79" s="37" t="inlineStr">
+      <c r="C79" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Use the sample conversation topic. Respond to a common objection. (th study 3)
 </t>
         </is>
       </c>
-      <c r="D79" s="34" t="n">
+      <c r="D79" s="35" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="27" t="n"/>
-      <c r="B80" s="35" t="n"/>
-      <c r="C80" s="27" t="n"/>
-      <c r="D80" s="36" t="n"/>
+      <c r="A80" s="30" t="n"/>
+      <c r="B80" s="36" t="n"/>
+      <c r="C80" s="30" t="n"/>
+      <c r="D80" s="37" t="n"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="32" t="inlineStr">
+      <c r="A81" s="33" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B81" s="15" t="n"/>
-      <c r="C81" s="37" t="inlineStr">
+      <c r="C81" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Why Study the Bible? (th study 14)
 </t>
         </is>
       </c>
-      <c r="D81" s="34" t="n">
+      <c r="D81" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="27" t="n"/>
-      <c r="B82" s="35" t="n"/>
-      <c r="C82" s="27" t="n"/>
-      <c r="D82" s="36" t="n"/>
+      <c r="A82" s="30" t="n"/>
+      <c r="B82" s="36" t="n"/>
+      <c r="C82" s="30" t="n"/>
+      <c r="D82" s="37" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" s="32" t="inlineStr">
+      <c r="A83" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B83" s="15" t="n"/>
-      <c r="C83" s="33" t="inlineStr">
+      <c r="C83" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 summary, review, and goal (th study 9)
 </t>
         </is>
       </c>
-      <c r="D83" s="34" t="n">
+      <c r="D83" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="27" t="n"/>
-      <c r="B84" s="35" t="n"/>
-      <c r="C84" s="27" t="n"/>
-      <c r="D84" s="36" t="n"/>
+      <c r="A84" s="30" t="n"/>
+      <c r="B84" s="36" t="n"/>
+      <c r="C84" s="30" t="n"/>
+      <c r="D84" s="37" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="15" t="n"/>
@@ -1855,7 +1865,7 @@
         </is>
       </c>
       <c r="B86" s="15" t="n"/>
-      <c r="C86" s="38" t="inlineStr">
+      <c r="C86" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -1868,8 +1878,8 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B87" s="27" t="n"/>
-      <c r="C87" s="30" t="inlineStr">
+      <c r="B87" s="30" t="n"/>
+      <c r="C87" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">“Prepare Now for a Medical Emergency”:  Discussion and video. To be handled by an elder. Allow time for several comments after the video.
 </t>
@@ -1885,7 +1895,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B88" s="27" t="n"/>
+      <c r="B88" s="30" t="n"/>
       <c r="C88" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 35
@@ -1902,11 +1912,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B89" s="27" t="n"/>
+      <c r="B89" s="30" t="n"/>
       <c r="C89" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-7</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D89" s="29" t="n">
@@ -1914,39 +1924,39 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="39" t="inlineStr">
+      <c r="A90" s="40" t="inlineStr">
         <is>
           <t>Song 88</t>
         </is>
       </c>
-      <c r="B90" s="27" t="n"/>
-      <c r="C90" s="40" t="inlineStr">
+      <c r="B90" s="30" t="n"/>
+      <c r="C90" s="41" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D90" s="36" t="n"/>
+      <c r="D90" s="37" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="15" t="n"/>
       <c r="B91" s="15" t="n"/>
-      <c r="C91" s="41" t="n"/>
+      <c r="C91" s="42" t="n"/>
       <c r="D91" s="15" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="15" t="n"/>
       <c r="B92" s="15" t="n"/>
-      <c r="C92" s="41" t="n"/>
+      <c r="C92" s="42" t="n"/>
       <c r="D92" s="15" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="15" t="n"/>
-      <c r="B93" s="42" t="inlineStr">
+      <c r="B93" s="43" t="inlineStr">
         <is>
           <t>Life and Ministry Meeting Workbook, February 2023</t>
         </is>
       </c>
-      <c r="C93" s="43" t="n"/>
+      <c r="C93" s="44" t="n"/>
       <c r="D93" s="15" t="n"/>
     </row>
     <row r="94">
@@ -1955,7 +1965,7 @@
           <t>Week 1</t>
         </is>
       </c>
-      <c r="B94" s="44" t="inlineStr">
+      <c r="B94" s="45" t="inlineStr">
         <is>
           <t>January 30 - February 5</t>
         </is>
@@ -2013,11 +2023,11 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B98" s="27" t="n"/>
+      <c r="B98" s="30" t="n"/>
       <c r="C98" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-8</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D98" s="29" t="n">
@@ -2030,7 +2040,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B99" s="27" t="n"/>
+      <c r="B99" s="30" t="n"/>
       <c r="C99" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“You Can Fulfill Challenging Assignments With Jehovah’s Help”: 
@@ -2047,8 +2057,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B100" s="27" t="n"/>
-      <c r="C100" s="30" t="inlineStr">
+      <c r="B100" s="30" t="n"/>
+      <c r="C100" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 9:33 —How does this verse help us to appreciate the importance of music in true worship? (w10 12/15 21 ¶6)
 </t>
@@ -2064,7 +2074,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B101" s="27" t="n"/>
+      <c r="B101" s="30" t="n"/>
       <c r="C101" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 7:1-13 (th study 10)
@@ -2084,7 +2094,7 @@
     <row r="103">
       <c r="A103" s="15" t="n"/>
       <c r="B103" s="15" t="n"/>
-      <c r="C103" s="31" t="inlineStr">
+      <c r="C103" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -2092,73 +2102,73 @@
       <c r="D103" s="25" t="n"/>
     </row>
     <row r="104">
-      <c r="A104" s="32" t="inlineStr">
+      <c r="A104" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B104" s="15" t="n"/>
-      <c r="C104" s="37" t="inlineStr">
+      <c r="C104" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Leave a jw.org contact card. (th study 16)
 </t>
         </is>
       </c>
-      <c r="D104" s="34" t="n">
+      <c r="D104" s="35" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="27" t="n"/>
-      <c r="B105" s="35" t="n"/>
-      <c r="C105" s="27" t="n"/>
-      <c r="D105" s="36" t="n"/>
+      <c r="A105" s="30" t="n"/>
+      <c r="B105" s="36" t="n"/>
+      <c r="C105" s="30" t="n"/>
+      <c r="D105" s="37" t="n"/>
     </row>
     <row r="106">
-      <c r="A106" s="32" t="inlineStr">
+      <c r="A106" s="33" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B106" s="15" t="n"/>
-      <c r="C106" s="37" t="inlineStr">
+      <c r="C106" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 20)
 </t>
         </is>
       </c>
-      <c r="D106" s="34" t="n">
+      <c r="D106" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="27" t="n"/>
-      <c r="B107" s="35" t="n"/>
-      <c r="C107" s="27" t="n"/>
-      <c r="D107" s="36" t="n"/>
+      <c r="A107" s="30" t="n"/>
+      <c r="B107" s="36" t="n"/>
+      <c r="C107" s="30" t="n"/>
+      <c r="D107" s="37" t="n"/>
     </row>
     <row r="108">
-      <c r="A108" s="32" t="inlineStr">
+      <c r="A108" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B108" s="15" t="n"/>
-      <c r="C108" s="37" t="inlineStr">
+      <c r="C108" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w21.06 3-4 ¶3-8 —Theme: Help Your Bible Student to Apply What He Is Learning. (th study 13)
 </t>
         </is>
       </c>
-      <c r="D108" s="34" t="n">
+      <c r="D108" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="27" t="n"/>
-      <c r="B109" s="35" t="n"/>
-      <c r="C109" s="27" t="n"/>
-      <c r="D109" s="36" t="n"/>
+      <c r="A109" s="30" t="n"/>
+      <c r="B109" s="36" t="n"/>
+      <c r="C109" s="30" t="n"/>
+      <c r="D109" s="37" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="15" t="n"/>
@@ -2173,7 +2183,7 @@
         </is>
       </c>
       <c r="B111" s="15" t="n"/>
-      <c r="C111" s="38" t="inlineStr">
+      <c r="C111" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -2186,7 +2196,7 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B112" s="27" t="n"/>
+      <c r="B112" s="30" t="n"/>
       <c r="C112" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Jehovah Helps Us Through Our Trials”:  Discussion and video.
@@ -2203,7 +2213,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B113" s="27" t="n"/>
+      <c r="B113" s="30" t="n"/>
       <c r="C113" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 36
@@ -2220,11 +2230,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B114" s="27" t="n"/>
+      <c r="B114" s="30" t="n"/>
       <c r="C114" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-9</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D114" s="29" t="n">
@@ -2315,11 +2325,11 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B121" s="27" t="n"/>
+      <c r="B121" s="30" t="n"/>
       <c r="C121" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-10</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D121" s="29" t="n">
@@ -2332,7 +2342,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B122" s="27" t="n"/>
+      <c r="B122" s="30" t="n"/>
       <c r="C122" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Desire to Do God’s Will”: 
@@ -2349,8 +2359,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B123" s="27" t="n"/>
-      <c r="C123" s="30" t="inlineStr">
+      <c r="B123" s="30" t="n"/>
+      <c r="C123" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 12:33 —What good example did the 50,000 men of Zebulun set? (it-1 1058 ¶5-6)
 </t>
@@ -2366,7 +2376,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B124" s="27" t="n"/>
+      <c r="B124" s="30" t="n"/>
       <c r="C124" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 11:26-47 (th study 5)
@@ -2386,7 +2396,7 @@
     <row r="126">
       <c r="A126" s="15" t="n"/>
       <c r="B126" s="15" t="n"/>
-      <c r="C126" s="31" t="inlineStr">
+      <c r="C126" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -2394,73 +2404,73 @@
       <c r="D126" s="25" t="n"/>
     </row>
     <row r="127">
-      <c r="A127" s="32" t="inlineStr">
+      <c r="A127" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B127" s="15" t="n"/>
-      <c r="C127" s="37" t="inlineStr">
+      <c r="C127" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a Bible study. (th study 12)
 </t>
         </is>
       </c>
-      <c r="D127" s="34" t="n">
+      <c r="D127" s="35" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="27" t="n"/>
-      <c r="B128" s="35" t="n"/>
-      <c r="C128" s="27" t="n"/>
-      <c r="D128" s="36" t="n"/>
+      <c r="A128" s="30" t="n"/>
+      <c r="B128" s="36" t="n"/>
+      <c r="C128" s="30" t="n"/>
+      <c r="D128" s="37" t="n"/>
     </row>
     <row r="129">
-      <c r="A129" s="32" t="inlineStr">
+      <c r="A129" s="33" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B129" s="15" t="n"/>
-      <c r="C129" s="37" t="inlineStr">
+      <c r="C129" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video What Happens at a Bible Study? (th study 6)
 </t>
         </is>
       </c>
-      <c r="D129" s="34" t="n">
+      <c r="D129" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="27" t="n"/>
-      <c r="B130" s="35" t="n"/>
-      <c r="C130" s="27" t="n"/>
-      <c r="D130" s="36" t="n"/>
+      <c r="A130" s="30" t="n"/>
+      <c r="B130" s="36" t="n"/>
+      <c r="C130" s="30" t="n"/>
+      <c r="D130" s="37" t="n"/>
     </row>
     <row r="131">
-      <c r="A131" s="32" t="inlineStr">
+      <c r="A131" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B131" s="15" t="n"/>
-      <c r="C131" s="33" t="inlineStr">
+      <c r="C131" s="34" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 09 intro and points 1-3 (th study 18)
 </t>
         </is>
       </c>
-      <c r="D131" s="34" t="n">
+      <c r="D131" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="27" t="n"/>
-      <c r="B132" s="35" t="n"/>
-      <c r="C132" s="27" t="n"/>
-      <c r="D132" s="36" t="n"/>
+      <c r="A132" s="30" t="n"/>
+      <c r="B132" s="36" t="n"/>
+      <c r="C132" s="30" t="n"/>
+      <c r="D132" s="37" t="n"/>
     </row>
     <row r="133">
       <c r="A133" s="15" t="n"/>
@@ -2475,7 +2485,7 @@
         </is>
       </c>
       <c r="B134" s="15" t="n"/>
-      <c r="C134" s="38" t="inlineStr">
+      <c r="C134" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -2488,7 +2498,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B135" s="27" t="n"/>
+      <c r="B135" s="30" t="n"/>
       <c r="C135" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Search for God’s Thinking”:  Discussion and video.
@@ -2505,7 +2515,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B136" s="27" t="n"/>
+      <c r="B136" s="30" t="n"/>
       <c r="C136" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Set Goals for the Memorial Season”:  Discussion.
@@ -2522,7 +2532,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B137" s="27" t="n"/>
+      <c r="B137" s="30" t="n"/>
       <c r="C137" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 points 1-5
@@ -2539,11 +2549,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B138" s="27" t="n"/>
+      <c r="B138" s="30" t="n"/>
       <c r="C138" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-11</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D138" s="29" t="n">
@@ -2634,11 +2644,11 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B145" s="27" t="n"/>
+      <c r="B145" s="30" t="n"/>
       <c r="C145" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-12</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D145" s="29" t="n">
@@ -2651,7 +2661,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B146" s="27" t="n"/>
+      <c r="B146" s="30" t="n"/>
       <c r="C146" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Following Direction Leads to Success”: 
@@ -2668,8 +2678,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B147" s="27" t="n"/>
-      <c r="C147" s="30" t="inlineStr">
+      <c r="B147" s="30" t="n"/>
+      <c r="C147" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 16:31 —Why could the Levites sing: “Jehovah has become King!”? (w14 1/15 10 ¶14)
 </t>
@@ -2685,7 +2695,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B148" s="27" t="n"/>
+      <c r="B148" s="30" t="n"/>
       <c r="C148" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 13:1-14 (th study 11)
@@ -2705,7 +2715,7 @@
     <row r="150">
       <c r="A150" s="15" t="n"/>
       <c r="B150" s="15" t="n"/>
-      <c r="C150" s="31" t="inlineStr">
+      <c r="C150" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -2713,73 +2723,73 @@
       <c r="D150" s="25" t="n"/>
     </row>
     <row r="151">
-      <c r="A151" s="32" t="inlineStr">
+      <c r="A151" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B151" s="15" t="n"/>
-      <c r="C151" s="37" t="inlineStr">
+      <c r="C151" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Respond to a common objection. (th study 18)
 </t>
         </is>
       </c>
-      <c r="D151" s="34" t="n">
+      <c r="D151" s="35" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="27" t="n"/>
-      <c r="B152" s="35" t="n"/>
-      <c r="C152" s="27" t="n"/>
-      <c r="D152" s="36" t="n"/>
+      <c r="A152" s="30" t="n"/>
+      <c r="B152" s="36" t="n"/>
+      <c r="C152" s="30" t="n"/>
+      <c r="D152" s="37" t="n"/>
     </row>
     <row r="153">
-      <c r="A153" s="32" t="inlineStr">
+      <c r="A153" s="33" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B153" s="15" t="n"/>
-      <c r="C153" s="37" t="inlineStr">
+      <c r="C153" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 7)
 </t>
         </is>
       </c>
-      <c r="D153" s="34" t="n">
+      <c r="D153" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="27" t="n"/>
-      <c r="B154" s="35" t="n"/>
-      <c r="C154" s="27" t="n"/>
-      <c r="D154" s="36" t="n"/>
+      <c r="A154" s="30" t="n"/>
+      <c r="B154" s="36" t="n"/>
+      <c r="C154" s="30" t="n"/>
+      <c r="D154" s="37" t="n"/>
     </row>
     <row r="155">
-      <c r="A155" s="32" t="inlineStr">
+      <c r="A155" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B155" s="15" t="n"/>
-      <c r="C155" s="37" t="inlineStr">
+      <c r="C155" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w16.01 13-14 ¶7-10 —Theme: “The Love the Christ Has Compels Us.” —2Co 5:14. (th study 8)
 </t>
         </is>
       </c>
-      <c r="D155" s="34" t="n">
+      <c r="D155" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="27" t="n"/>
-      <c r="B156" s="35" t="n"/>
-      <c r="C156" s="27" t="n"/>
-      <c r="D156" s="36" t="n"/>
+      <c r="A156" s="30" t="n"/>
+      <c r="B156" s="36" t="n"/>
+      <c r="C156" s="30" t="n"/>
+      <c r="D156" s="37" t="n"/>
     </row>
     <row r="157">
       <c r="A157" s="15" t="n"/>
@@ -2794,7 +2804,7 @@
         </is>
       </c>
       <c r="B158" s="15" t="n"/>
-      <c r="C158" s="38" t="inlineStr">
+      <c r="C158" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -2807,8 +2817,8 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B159" s="27" t="n"/>
-      <c r="C159" s="30" t="inlineStr">
+      <c r="B159" s="30" t="n"/>
+      <c r="C159" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Become Jehovah’s Friend —Pay Attention at the Meetings:  Discussion. Play the video. Then, if possible, ask selected children: Why should we pay attention at meetings? What can help you to do so?
 </t>
@@ -2824,7 +2834,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B160" s="27" t="n"/>
+      <c r="B160" s="30" t="n"/>
       <c r="C160" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
@@ -2841,8 +2851,8 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B161" s="27" t="n"/>
-      <c r="C161" s="30" t="inlineStr">
+      <c r="B161" s="30" t="n"/>
+      <c r="C161" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 point 6 and summary, review, and goal
 </t>
@@ -2858,11 +2868,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B162" s="27" t="n"/>
+      <c r="B162" s="30" t="n"/>
       <c r="C162" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-13</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D162" s="29" t="n">
@@ -2953,11 +2963,11 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B169" s="27" t="n"/>
+      <c r="B169" s="30" t="n"/>
       <c r="C169" s="28" t="inlineStr">
         <is>
-          <t>Opening Comments 
-14</t>
+          <t xml:space="preserve">Opening Comments 
+ </t>
         </is>
       </c>
       <c r="D169" s="29" t="n">
@@ -2970,7 +2980,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B170" s="27" t="n"/>
+      <c r="B170" s="30" t="n"/>
       <c r="C170" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Maintain Your Joy Despite Disappointments”: 
@@ -2987,8 +2997,8 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B171" s="27" t="n"/>
-      <c r="C171" s="30" t="inlineStr">
+      <c r="B171" s="30" t="n"/>
+      <c r="C171" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 17:16-18 —Like David, of what can we be confident? (w20.02 12, box)
 </t>
@@ -3004,7 +3014,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B172" s="27" t="n"/>
+      <c r="B172" s="30" t="n"/>
       <c r="C172" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 18:1-17 (th study 2)
@@ -3024,7 +3034,7 @@
     <row r="174">
       <c r="A174" s="15" t="n"/>
       <c r="B174" s="15" t="n"/>
-      <c r="C174" s="31" t="inlineStr">
+      <c r="C174" s="32" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
@@ -3032,73 +3042,73 @@
       <c r="D174" s="25" t="n"/>
     </row>
     <row r="175">
-      <c r="A175" s="32" t="inlineStr">
+      <c r="A175" s="33" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B175" s="15" t="n"/>
-      <c r="C175" s="37" t="inlineStr">
+      <c r="C175" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Jehovah’s Witnesses —Who Are We? (th study 17)
 </t>
         </is>
       </c>
-      <c r="D175" s="34" t="n">
+      <c r="D175" s="35" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="27" t="n"/>
-      <c r="B176" s="35" t="n"/>
-      <c r="C176" s="27" t="n"/>
-      <c r="D176" s="36" t="n"/>
+      <c r="A176" s="30" t="n"/>
+      <c r="B176" s="36" t="n"/>
+      <c r="C176" s="30" t="n"/>
+      <c r="D176" s="37" t="n"/>
     </row>
     <row r="177">
-      <c r="A177" s="32" t="inlineStr">
+      <c r="A177" s="33" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B177" s="15" t="n"/>
-      <c r="C177" s="37" t="inlineStr">
+      <c r="C177" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 3)
 </t>
         </is>
       </c>
-      <c r="D177" s="34" t="n">
+      <c r="D177" s="35" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="27" t="n"/>
-      <c r="B178" s="35" t="n"/>
-      <c r="C178" s="27" t="n"/>
-      <c r="D178" s="36" t="n"/>
+      <c r="A178" s="30" t="n"/>
+      <c r="B178" s="36" t="n"/>
+      <c r="C178" s="30" t="n"/>
+      <c r="D178" s="37" t="n"/>
     </row>
     <row r="179">
-      <c r="A179" s="32" t="inlineStr">
+      <c r="A179" s="33" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B179" s="15" t="n"/>
-      <c r="C179" s="33" t="inlineStr">
+      <c r="C179" s="34" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 09 point 4 (th study 9)
 </t>
         </is>
       </c>
-      <c r="D179" s="34" t="n">
+      <c r="D179" s="35" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="27" t="n"/>
-      <c r="B180" s="35" t="n"/>
-      <c r="C180" s="27" t="n"/>
-      <c r="D180" s="36" t="n"/>
+      <c r="A180" s="30" t="n"/>
+      <c r="B180" s="36" t="n"/>
+      <c r="C180" s="30" t="n"/>
+      <c r="D180" s="37" t="n"/>
     </row>
     <row r="181">
       <c r="A181" s="15" t="n"/>
@@ -3113,7 +3123,7 @@
         </is>
       </c>
       <c r="B182" s="15" t="n"/>
-      <c r="C182" s="38" t="inlineStr">
+      <c r="C182" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -3126,8 +3136,8 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B183" s="27" t="n"/>
-      <c r="C183" s="30" t="inlineStr">
+      <c r="B183" s="30" t="n"/>
+      <c r="C183" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Annual Service Report:  Discussion. After reading the announcement from the branch office regarding the annual service report, invite the audience to highlight other positive aspects of the 2022 Service Year Report of Jehovah’s Witnesses Worldwide. Interview publishers, selected in advance, who had encouraging experiences in the ministry during the past year.
 </t>
@@ -3143,7 +3153,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B184" s="27" t="n"/>
+      <c r="B184" s="30" t="n"/>
       <c r="C184" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 38 points 1-4
@@ -3160,11 +3170,11 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B185" s="27" t="n"/>
+      <c r="B185" s="30" t="n"/>
       <c r="C185" s="28" t="inlineStr">
         <is>
-          <t>Concluding Comments 
-15</t>
+          <t xml:space="preserve">Concluding Comments 
+ </t>
         </is>
       </c>
       <c r="D185" s="29" t="n">
@@ -3178,18 +3188,18 @@
       <c r="D186" s="25" t="n"/>
     </row>
     <row r="187">
-      <c r="A187" s="39" t="inlineStr">
+      <c r="A187" s="40" t="inlineStr">
         <is>
           <t>Song 141</t>
         </is>
       </c>
-      <c r="B187" s="27" t="n"/>
-      <c r="C187" s="40" t="inlineStr">
+      <c r="B187" s="30" t="n"/>
+      <c r="C187" s="41" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D187" s="36" t="n"/>
+      <c r="D187" s="37" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added csv and updated auto complete
</commit_message>
<xml_diff>
--- a/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
+++ b/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
@@ -295,16 +295,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -807,11 +807,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B6" s="27" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
+      <c r="B6" s="27" t="n"/>
       <c r="C6" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -828,7 +824,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B7" s="30" t="n"/>
+      <c r="B7" s="27" t="n"/>
       <c r="C7" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Why Be Humble?”: 
@@ -845,7 +841,11 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B8" s="30" t="n"/>
+      <c r="B8" s="30" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="C8" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  2Ki 23:24, 25 —What encouragement does Josiah’s example provide for those who have endured a difficult childhood? (w01 4/15 26 ¶3-4)
@@ -862,7 +862,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B9" s="30" t="n"/>
+      <c r="B9" s="27" t="n"/>
       <c r="C9" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 23:16-25 (th study 2)
@@ -895,7 +895,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B12" s="30" t="n"/>
+      <c r="B12" s="27" t="n"/>
       <c r="C12" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call Video:  Discussion. Play the video Initial Call: Prayer —Ps 65:2. Stop the video at each pause, and ask the audience the questions that appear in the video.
@@ -924,9 +924,9 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="30" t="n"/>
+      <c r="A14" s="27" t="n"/>
       <c r="B14" s="36" t="n"/>
-      <c r="C14" s="30" t="n"/>
+      <c r="C14" s="27" t="n"/>
       <c r="D14" s="37" t="n"/>
     </row>
     <row r="15">
@@ -947,9 +947,9 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="30" t="n"/>
+      <c r="A16" s="27" t="n"/>
       <c r="B16" s="36" t="n"/>
-      <c r="C16" s="30" t="n"/>
+      <c r="C16" s="27" t="n"/>
       <c r="D16" s="37" t="n"/>
     </row>
     <row r="17">
@@ -978,7 +978,7 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B19" s="30" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Humble or Haughty? (Jas 4:6):  Discussion. Play the video. Then ask the audience: What is the difference between humility and haughtiness? What can we learn from Moses’ example? Why are you determined to remain humble?
@@ -995,7 +995,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B20" s="30" t="n"/>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 33
@@ -1012,7 +1012,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B21" s="30" t="n"/>
+      <c r="B21" s="27" t="n"/>
       <c r="C21" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -1107,7 +1107,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B28" s="30" t="n"/>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -1124,7 +1124,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B29" s="30" t="n"/>
+      <c r="B29" s="27" t="n"/>
       <c r="C29" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Maintain Your Sense of Urgency”: 
@@ -1141,7 +1141,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B30" s="30" t="n"/>
+      <c r="B30" s="27" t="n"/>
       <c r="C30" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  2Ki 24:3, 4 —What do these verses teach us about Jehovah? (w05 8/1 12 ¶1)
@@ -1158,7 +1158,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B31" s="30" t="n"/>
+      <c r="B31" s="27" t="n"/>
       <c r="C31" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 24:1-17 (th study 11)
@@ -1191,7 +1191,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B34" s="30" t="n"/>
+      <c r="B34" s="27" t="n"/>
       <c r="C34" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit Video:  Discussion. Play the video Return Visit: Prayer —1Jo 5:14. Stop the video at each pause, and ask the audience the questions that appear in the video.
@@ -1220,9 +1220,9 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="30" t="n"/>
+      <c r="A36" s="27" t="n"/>
       <c r="B36" s="36" t="n"/>
-      <c r="C36" s="30" t="n"/>
+      <c r="C36" s="27" t="n"/>
       <c r="D36" s="37" t="n"/>
     </row>
     <row r="37">
@@ -1243,9 +1243,9 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="30" t="n"/>
+      <c r="A38" s="27" t="n"/>
       <c r="B38" s="36" t="n"/>
-      <c r="C38" s="30" t="n"/>
+      <c r="C38" s="27" t="n"/>
       <c r="D38" s="37" t="n"/>
     </row>
     <row r="39">
@@ -1274,7 +1274,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B41" s="30" t="n"/>
+      <c r="B41" s="27" t="n"/>
       <c r="C41" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
@@ -1291,7 +1291,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B42" s="30" t="n"/>
+      <c r="B42" s="27" t="n"/>
       <c r="C42" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff section 2 review
@@ -1308,7 +1308,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B43" s="30" t="n"/>
+      <c r="B43" s="27" t="n"/>
       <c r="C43" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -1403,7 +1403,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B50" s="30" t="n"/>
+      <c r="B50" s="27" t="n"/>
       <c r="C50" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -1420,7 +1420,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B51" s="30" t="n"/>
+      <c r="B51" s="27" t="n"/>
       <c r="C51" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“The Bible —A Book of Fact, Not Fiction”: 
@@ -1437,7 +1437,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B52" s="30" t="n"/>
+      <c r="B52" s="27" t="n"/>
       <c r="C52" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 3:1-3 —Why were women occasionally named in genealogical registers? (it-1 911 ¶3-4)
@@ -1454,7 +1454,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B53" s="30" t="n"/>
+      <c r="B53" s="27" t="n"/>
       <c r="C53" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 1:43-54 (th study 5)
@@ -1499,9 +1499,9 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="30" t="n"/>
+      <c r="A57" s="27" t="n"/>
       <c r="B57" s="36" t="n"/>
-      <c r="C57" s="30" t="n"/>
+      <c r="C57" s="27" t="n"/>
       <c r="D57" s="37" t="n"/>
     </row>
     <row r="58">
@@ -1522,9 +1522,9 @@
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="30" t="n"/>
+      <c r="A59" s="27" t="n"/>
       <c r="B59" s="36" t="n"/>
-      <c r="C59" s="30" t="n"/>
+      <c r="C59" s="27" t="n"/>
       <c r="D59" s="37" t="n"/>
     </row>
     <row r="60">
@@ -1545,9 +1545,9 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="30" t="n"/>
+      <c r="A61" s="27" t="n"/>
       <c r="B61" s="36" t="n"/>
-      <c r="C61" s="30" t="n"/>
+      <c r="C61" s="27" t="n"/>
       <c r="D61" s="37" t="n"/>
     </row>
     <row r="62">
@@ -1576,7 +1576,7 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B64" s="30" t="n"/>
+      <c r="B64" s="27" t="n"/>
       <c r="C64" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Faith in God’s Word”:  Discussion and video.
@@ -1593,7 +1593,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B65" s="30" t="n"/>
+      <c r="B65" s="27" t="n"/>
       <c r="C65" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 34
@@ -1610,7 +1610,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B66" s="30" t="n"/>
+      <c r="B66" s="27" t="n"/>
       <c r="C66" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -1705,7 +1705,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B73" s="30" t="n"/>
+      <c r="B73" s="27" t="n"/>
       <c r="C73" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -1722,7 +1722,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B74" s="30" t="n"/>
+      <c r="B74" s="27" t="n"/>
       <c r="C74" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“What Do My Prayers Reveal About Me?”: 
@@ -1739,7 +1739,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B75" s="30" t="n"/>
+      <c r="B75" s="27" t="n"/>
       <c r="C75" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 5:10 —How can the victory over the Hagrites encourage us when we face seemingly insurmountable obstacles? (w05 10/1 9 ¶7)
@@ -1756,7 +1756,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B76" s="30" t="n"/>
+      <c r="B76" s="27" t="n"/>
       <c r="C76" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 6:61-81 (th study 2)
@@ -1801,9 +1801,9 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="30" t="n"/>
+      <c r="A80" s="27" t="n"/>
       <c r="B80" s="36" t="n"/>
-      <c r="C80" s="30" t="n"/>
+      <c r="C80" s="27" t="n"/>
       <c r="D80" s="37" t="n"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
@@ -1824,9 +1824,9 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="30" t="n"/>
+      <c r="A82" s="27" t="n"/>
       <c r="B82" s="36" t="n"/>
-      <c r="C82" s="30" t="n"/>
+      <c r="C82" s="27" t="n"/>
       <c r="D82" s="37" t="n"/>
     </row>
     <row r="83">
@@ -1847,9 +1847,9 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="30" t="n"/>
+      <c r="A84" s="27" t="n"/>
       <c r="B84" s="36" t="n"/>
-      <c r="C84" s="30" t="n"/>
+      <c r="C84" s="27" t="n"/>
       <c r="D84" s="37" t="n"/>
     </row>
     <row r="85">
@@ -1878,7 +1878,7 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B87" s="30" t="n"/>
+      <c r="B87" s="27" t="n"/>
       <c r="C87" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">“Prepare Now for a Medical Emergency”:  Discussion and video. To be handled by an elder. Allow time for several comments after the video.
@@ -1895,7 +1895,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B88" s="30" t="n"/>
+      <c r="B88" s="27" t="n"/>
       <c r="C88" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 35
@@ -1912,7 +1912,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B89" s="30" t="n"/>
+      <c r="B89" s="27" t="n"/>
       <c r="C89" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -1929,7 +1929,7 @@
           <t>Song 88</t>
         </is>
       </c>
-      <c r="B90" s="30" t="n"/>
+      <c r="B90" s="27" t="n"/>
       <c r="C90" s="41" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
@@ -2023,7 +2023,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B98" s="30" t="n"/>
+      <c r="B98" s="27" t="n"/>
       <c r="C98" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -2040,7 +2040,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B99" s="30" t="n"/>
+      <c r="B99" s="27" t="n"/>
       <c r="C99" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“You Can Fulfill Challenging Assignments With Jehovah’s Help”: 
@@ -2057,7 +2057,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B100" s="30" t="n"/>
+      <c r="B100" s="27" t="n"/>
       <c r="C100" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 9:33 —How does this verse help us to appreciate the importance of music in true worship? (w10 12/15 21 ¶6)
@@ -2074,7 +2074,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B101" s="30" t="n"/>
+      <c r="B101" s="27" t="n"/>
       <c r="C101" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 7:1-13 (th study 10)
@@ -2119,9 +2119,9 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="30" t="n"/>
+      <c r="A105" s="27" t="n"/>
       <c r="B105" s="36" t="n"/>
-      <c r="C105" s="30" t="n"/>
+      <c r="C105" s="27" t="n"/>
       <c r="D105" s="37" t="n"/>
     </row>
     <row r="106">
@@ -2142,9 +2142,9 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="30" t="n"/>
+      <c r="A107" s="27" t="n"/>
       <c r="B107" s="36" t="n"/>
-      <c r="C107" s="30" t="n"/>
+      <c r="C107" s="27" t="n"/>
       <c r="D107" s="37" t="n"/>
     </row>
     <row r="108">
@@ -2165,9 +2165,9 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="30" t="n"/>
+      <c r="A109" s="27" t="n"/>
       <c r="B109" s="36" t="n"/>
-      <c r="C109" s="30" t="n"/>
+      <c r="C109" s="27" t="n"/>
       <c r="D109" s="37" t="n"/>
     </row>
     <row r="110">
@@ -2196,7 +2196,7 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B112" s="30" t="n"/>
+      <c r="B112" s="27" t="n"/>
       <c r="C112" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Jehovah Helps Us Through Our Trials”:  Discussion and video.
@@ -2213,7 +2213,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B113" s="30" t="n"/>
+      <c r="B113" s="27" t="n"/>
       <c r="C113" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 36
@@ -2230,7 +2230,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B114" s="30" t="n"/>
+      <c r="B114" s="27" t="n"/>
       <c r="C114" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -2325,7 +2325,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B121" s="30" t="n"/>
+      <c r="B121" s="27" t="n"/>
       <c r="C121" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -2342,7 +2342,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B122" s="30" t="n"/>
+      <c r="B122" s="27" t="n"/>
       <c r="C122" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Desire to Do God’s Will”: 
@@ -2359,7 +2359,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B123" s="30" t="n"/>
+      <c r="B123" s="27" t="n"/>
       <c r="C123" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 12:33 —What good example did the 50,000 men of Zebulun set? (it-1 1058 ¶5-6)
@@ -2376,7 +2376,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B124" s="30" t="n"/>
+      <c r="B124" s="27" t="n"/>
       <c r="C124" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 11:26-47 (th study 5)
@@ -2421,9 +2421,9 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="30" t="n"/>
+      <c r="A128" s="27" t="n"/>
       <c r="B128" s="36" t="n"/>
-      <c r="C128" s="30" t="n"/>
+      <c r="C128" s="27" t="n"/>
       <c r="D128" s="37" t="n"/>
     </row>
     <row r="129">
@@ -2444,9 +2444,9 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="30" t="n"/>
+      <c r="A130" s="27" t="n"/>
       <c r="B130" s="36" t="n"/>
-      <c r="C130" s="30" t="n"/>
+      <c r="C130" s="27" t="n"/>
       <c r="D130" s="37" t="n"/>
     </row>
     <row r="131">
@@ -2467,9 +2467,9 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="30" t="n"/>
+      <c r="A132" s="27" t="n"/>
       <c r="B132" s="36" t="n"/>
-      <c r="C132" s="30" t="n"/>
+      <c r="C132" s="27" t="n"/>
       <c r="D132" s="37" t="n"/>
     </row>
     <row r="133">
@@ -2498,7 +2498,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B135" s="30" t="n"/>
+      <c r="B135" s="27" t="n"/>
       <c r="C135" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Search for God’s Thinking”:  Discussion and video.
@@ -2515,7 +2515,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B136" s="30" t="n"/>
+      <c r="B136" s="27" t="n"/>
       <c r="C136" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Set Goals for the Memorial Season”:  Discussion.
@@ -2532,7 +2532,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B137" s="30" t="n"/>
+      <c r="B137" s="27" t="n"/>
       <c r="C137" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 points 1-5
@@ -2549,7 +2549,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B138" s="30" t="n"/>
+      <c r="B138" s="27" t="n"/>
       <c r="C138" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -2644,7 +2644,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B145" s="30" t="n"/>
+      <c r="B145" s="27" t="n"/>
       <c r="C145" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -2661,7 +2661,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B146" s="30" t="n"/>
+      <c r="B146" s="27" t="n"/>
       <c r="C146" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Following Direction Leads to Success”: 
@@ -2678,7 +2678,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B147" s="30" t="n"/>
+      <c r="B147" s="27" t="n"/>
       <c r="C147" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 16:31 —Why could the Levites sing: “Jehovah has become King!”? (w14 1/15 10 ¶14)
@@ -2695,7 +2695,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B148" s="30" t="n"/>
+      <c r="B148" s="27" t="n"/>
       <c r="C148" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 13:1-14 (th study 11)
@@ -2740,9 +2740,9 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="30" t="n"/>
+      <c r="A152" s="27" t="n"/>
       <c r="B152" s="36" t="n"/>
-      <c r="C152" s="30" t="n"/>
+      <c r="C152" s="27" t="n"/>
       <c r="D152" s="37" t="n"/>
     </row>
     <row r="153">
@@ -2763,9 +2763,9 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="30" t="n"/>
+      <c r="A154" s="27" t="n"/>
       <c r="B154" s="36" t="n"/>
-      <c r="C154" s="30" t="n"/>
+      <c r="C154" s="27" t="n"/>
       <c r="D154" s="37" t="n"/>
     </row>
     <row r="155">
@@ -2786,9 +2786,9 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="30" t="n"/>
+      <c r="A156" s="27" t="n"/>
       <c r="B156" s="36" t="n"/>
-      <c r="C156" s="30" t="n"/>
+      <c r="C156" s="27" t="n"/>
       <c r="D156" s="37" t="n"/>
     </row>
     <row r="157">
@@ -2817,7 +2817,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B159" s="30" t="n"/>
+      <c r="B159" s="27" t="n"/>
       <c r="C159" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Become Jehovah’s Friend —Pay Attention at the Meetings:  Discussion. Play the video. Then, if possible, ask selected children: Why should we pay attention at meetings? What can help you to do so?
@@ -2834,7 +2834,7 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B160" s="30" t="n"/>
+      <c r="B160" s="27" t="n"/>
       <c r="C160" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
@@ -2851,7 +2851,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B161" s="30" t="n"/>
+      <c r="B161" s="27" t="n"/>
       <c r="C161" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 point 6 and summary, review, and goal
@@ -2868,7 +2868,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B162" s="30" t="n"/>
+      <c r="B162" s="27" t="n"/>
       <c r="C162" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -2963,7 +2963,7 @@
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B169" s="30" t="n"/>
+      <c r="B169" s="27" t="n"/>
       <c r="C169" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
@@ -2980,7 +2980,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B170" s="30" t="n"/>
+      <c r="B170" s="27" t="n"/>
       <c r="C170" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">“Maintain Your Joy Despite Disappointments”: 
@@ -2997,7 +2997,7 @@
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B171" s="30" t="n"/>
+      <c r="B171" s="27" t="n"/>
       <c r="C171" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 17:16-18 —Like David, of what can we be confident? (w20.02 12, box)
@@ -3014,7 +3014,7 @@
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B172" s="30" t="n"/>
+      <c r="B172" s="27" t="n"/>
       <c r="C172" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 18:1-17 (th study 2)
@@ -3059,9 +3059,9 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="30" t="n"/>
+      <c r="A176" s="27" t="n"/>
       <c r="B176" s="36" t="n"/>
-      <c r="C176" s="30" t="n"/>
+      <c r="C176" s="27" t="n"/>
       <c r="D176" s="37" t="n"/>
     </row>
     <row r="177">
@@ -3082,9 +3082,9 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="30" t="n"/>
+      <c r="A178" s="27" t="n"/>
       <c r="B178" s="36" t="n"/>
-      <c r="C178" s="30" t="n"/>
+      <c r="C178" s="27" t="n"/>
       <c r="D178" s="37" t="n"/>
     </row>
     <row r="179">
@@ -3105,9 +3105,9 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="30" t="n"/>
+      <c r="A180" s="27" t="n"/>
       <c r="B180" s="36" t="n"/>
-      <c r="C180" s="30" t="n"/>
+      <c r="C180" s="27" t="n"/>
       <c r="D180" s="37" t="n"/>
     </row>
     <row r="181">
@@ -3136,7 +3136,7 @@
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B183" s="30" t="n"/>
+      <c r="B183" s="27" t="n"/>
       <c r="C183" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Annual Service Report:  Discussion. After reading the announcement from the branch office regarding the annual service report, invite the audience to highlight other positive aspects of the 2022 Service Year Report of Jehovah’s Witnesses Worldwide. Interview publishers, selected in advance, who had encouraging experiences in the ministry during the past year.
@@ -3153,7 +3153,7 @@
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B184" s="30" t="n"/>
+      <c r="B184" s="27" t="n"/>
       <c r="C184" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 38 points 1-4
@@ -3170,7 +3170,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B185" s="30" t="n"/>
+      <c r="B185" s="27" t="n"/>
       <c r="C185" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
@@ -3193,7 +3193,7 @@
           <t>Song 141</t>
         </is>
       </c>
-      <c r="B187" s="30" t="n"/>
+      <c r="B187" s="27" t="n"/>
       <c r="C187" s="41" t="inlineStr">
         <is>
           <t>Closing Prayer</t>

</xml_diff>

<commit_message>
Eye dropper tool correctly transfering to sheet
</commit_message>
<xml_diff>
--- a/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
+++ b/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
@@ -66,7 +66,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -95,6 +95,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF990000"/>
         <bgColor rgb="FF990000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f6a07a"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -276,11 +281,15 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -314,12 +323,18 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -765,13 +780,13 @@
           <t>Song 28</t>
         </is>
       </c>
-      <c r="B3" s="15" t="n"/>
-      <c r="C3" s="22" t="inlineStr">
+      <c r="B3" s="22" t="n"/>
+      <c r="C3" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D3" s="23" t="inlineStr">
+      <c r="D3" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -781,85 +796,85 @@
       <c r="A4" s="15" t="n"/>
       <c r="B4" s="15" t="n"/>
       <c r="C4" s="15" t="n"/>
-      <c r="D4" s="23" t="n">
+      <c r="D4" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="n"/>
       <c r="B5" s="15" t="n"/>
-      <c r="C5" s="24" t="inlineStr">
+      <c r="C5" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D5" s="25" t="n"/>
+      <c r="D5" s="27" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="26" t="inlineStr">
+      <c r="A6" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B6" s="27" t="n"/>
-      <c r="C6" s="28" t="inlineStr">
+      <c r="B6" s="29" t="n"/>
+      <c r="C6" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D6" s="29" t="n">
+      <c r="D6" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="26" t="inlineStr">
+      <c r="A7" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B7" s="27" t="n"/>
-      <c r="C7" s="28" t="inlineStr">
+      <c r="B7" s="29" t="n"/>
+      <c r="C7" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Why Be Humble?”: 
 </t>
         </is>
       </c>
-      <c r="D7" s="29" t="n">
+      <c r="D7" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="26" t="inlineStr">
+      <c r="A8" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B8" s="27" t="n"/>
-      <c r="C8" s="30" t="inlineStr">
+      <c r="B8" s="29" t="n"/>
+      <c r="C8" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  2Ki 23:24, 25 —What encouragement does Josiah’s example provide for those who have endured a difficult childhood? (w01 4/15 26 ¶3-4)
 </t>
         </is>
       </c>
-      <c r="D8" s="29" t="n">
+      <c r="D8" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="26" t="inlineStr">
+      <c r="A9" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B9" s="27" t="n"/>
-      <c r="C9" s="28" t="inlineStr">
+      <c r="B9" s="29" t="n"/>
+      <c r="C9" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 23:16-25 (th study 2)
 </t>
         </is>
       </c>
-      <c r="D9" s="29" t="n">
+      <c r="D9" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -867,171 +882,171 @@
       <c r="A10" s="15" t="n"/>
       <c r="B10" s="15" t="n"/>
       <c r="C10" s="15" t="inlineStr"/>
-      <c r="D10" s="25" t="n"/>
+      <c r="D10" s="27" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="15" t="n"/>
       <c r="B11" s="15" t="n"/>
-      <c r="C11" s="31" t="inlineStr">
+      <c r="C11" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D11" s="25" t="n"/>
+      <c r="D11" s="27" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="26" t="inlineStr">
+      <c r="A12" s="28" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B12" s="27" t="n"/>
-      <c r="C12" s="30" t="inlineStr">
+      <c r="B12" s="29" t="n"/>
+      <c r="C12" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call Video:  Discussion. Play the video Initial Call: Prayer —Ps 65:2. Stop the video at each pause, and ask the audience the questions that appear in the video.
 </t>
         </is>
       </c>
-      <c r="D12" s="29" t="n">
+      <c r="D12" s="31" t="n">
         <v>0.3173611111111111</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="32" t="inlineStr">
+      <c r="A13" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B13" s="15" t="n"/>
-      <c r="C13" s="33" t="inlineStr">
+      <c r="C13" s="35" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Use the sample conversation topic. (th study 1)
 </t>
         </is>
       </c>
-      <c r="D13" s="34" t="n">
+      <c r="D13" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="27" t="n"/>
-      <c r="B14" s="35" t="n"/>
-      <c r="C14" s="27" t="n"/>
-      <c r="D14" s="36" t="n"/>
+      <c r="A14" s="29" t="n"/>
+      <c r="B14" s="37" t="n"/>
+      <c r="C14" s="29" t="n"/>
+      <c r="D14" s="38" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="32" t="inlineStr">
+      <c r="A15" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B15" s="15" t="n"/>
-      <c r="C15" s="37" t="inlineStr">
+      <c r="C15" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 16)
 </t>
         </is>
       </c>
-      <c r="D15" s="34" t="n">
+      <c r="D15" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="27" t="n"/>
-      <c r="B16" s="35" t="n"/>
-      <c r="C16" s="27" t="n"/>
-      <c r="D16" s="36" t="n"/>
+      <c r="A16" s="29" t="n"/>
+      <c r="B16" s="37" t="n"/>
+      <c r="C16" s="29" t="n"/>
+      <c r="D16" s="38" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="15" t="n"/>
       <c r="B17" s="15" t="n"/>
       <c r="C17" s="15" t="inlineStr"/>
-      <c r="D17" s="25" t="n"/>
+      <c r="D17" s="27" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="21" t="inlineStr">
+      <c r="A18" s="40" t="inlineStr">
         <is>
           <t>Song 120</t>
         </is>
       </c>
       <c r="B18" s="15" t="n"/>
-      <c r="C18" s="38" t="inlineStr">
+      <c r="C18" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D18" s="25" t="n"/>
+      <c r="D18" s="27" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="26" t="inlineStr">
+      <c r="A19" s="28" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B19" s="27" t="n"/>
-      <c r="C19" s="30" t="inlineStr">
+      <c r="B19" s="29" t="n"/>
+      <c r="C19" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Humble or Haughty? (Jas 4:6):  Discussion. Play the video. Then ask the audience: What is the difference between humility and haughtiness? What can we learn from Moses’ example? Why are you determined to remain humble?
 </t>
         </is>
       </c>
-      <c r="D19" s="29" t="n">
+      <c r="D19" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="26" t="inlineStr">
+      <c r="A20" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B20" s="27" t="n"/>
-      <c r="C20" s="28" t="inlineStr">
+      <c r="B20" s="29" t="n"/>
+      <c r="C20" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 33
 </t>
         </is>
       </c>
-      <c r="D20" s="29" t="n">
+      <c r="D20" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="26" t="inlineStr">
+      <c r="A21" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B21" s="27" t="n"/>
-      <c r="C21" s="28" t="inlineStr">
+      <c r="B21" s="29" t="n"/>
+      <c r="C21" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D21" s="29" t="n">
+      <c r="D21" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="21" t="inlineStr">
+      <c r="A22" s="40" t="inlineStr">
         <is>
           <t>Song 23</t>
         </is>
       </c>
       <c r="B22" s="15" t="n"/>
-      <c r="C22" s="22" t="inlineStr">
+      <c r="C22" s="42" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D22" s="25" t="n"/>
+      <c r="D22" s="27" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="21" t="n"/>
+      <c r="A23" s="40" t="n"/>
       <c r="B23" s="15" t="n"/>
-      <c r="C23" s="22" t="n"/>
-      <c r="D23" s="25" t="n"/>
+      <c r="C23" s="42" t="n"/>
+      <c r="D23" s="27" t="n"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="17" t="inlineStr">
@@ -1061,13 +1076,13 @@
           <t>Song 60</t>
         </is>
       </c>
-      <c r="B25" s="15" t="n"/>
-      <c r="C25" s="22" t="inlineStr">
+      <c r="B25" s="22" t="n"/>
+      <c r="C25" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D25" s="23" t="inlineStr">
+      <c r="D25" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -1077,85 +1092,85 @@
       <c r="A26" s="15" t="n"/>
       <c r="B26" s="15" t="n"/>
       <c r="C26" s="15" t="n"/>
-      <c r="D26" s="23" t="n">
+      <c r="D26" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="15" t="n"/>
       <c r="B27" s="15" t="n"/>
-      <c r="C27" s="24" t="inlineStr">
+      <c r="C27" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D27" s="25" t="n"/>
+      <c r="D27" s="27" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="26" t="inlineStr">
+      <c r="A28" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B28" s="27" t="n"/>
-      <c r="C28" s="28" t="inlineStr">
+      <c r="B28" s="29" t="n"/>
+      <c r="C28" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D28" s="29" t="n">
+      <c r="D28" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="26" t="inlineStr">
+      <c r="A29" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B29" s="27" t="n"/>
-      <c r="C29" s="28" t="inlineStr">
+      <c r="B29" s="29" t="n"/>
+      <c r="C29" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Maintain Your Sense of Urgency”: 
 </t>
         </is>
       </c>
-      <c r="D29" s="29" t="n">
+      <c r="D29" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="26" t="inlineStr">
+      <c r="A30" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B30" s="27" t="n"/>
-      <c r="C30" s="30" t="inlineStr">
+      <c r="B30" s="29" t="n"/>
+      <c r="C30" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  2Ki 24:3, 4 —What do these verses teach us about Jehovah? (w05 8/1 12 ¶1)
 </t>
         </is>
       </c>
-      <c r="D30" s="29" t="n">
+      <c r="D30" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="26" t="inlineStr">
+      <c r="A31" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B31" s="27" t="n"/>
-      <c r="C31" s="28" t="inlineStr">
+      <c r="B31" s="29" t="n"/>
+      <c r="C31" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 24:1-17 (th study 11)
 </t>
         </is>
       </c>
-      <c r="D31" s="29" t="n">
+      <c r="D31" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -1163,171 +1178,171 @@
       <c r="A32" s="15" t="n"/>
       <c r="B32" s="15" t="n"/>
       <c r="C32" s="15" t="inlineStr"/>
-      <c r="D32" s="25" t="n"/>
+      <c r="D32" s="27" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="15" t="n"/>
       <c r="B33" s="15" t="n"/>
-      <c r="C33" s="31" t="inlineStr">
+      <c r="C33" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D33" s="25" t="n"/>
+      <c r="D33" s="27" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="26" t="inlineStr">
+      <c r="A34" s="28" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B34" s="27" t="n"/>
-      <c r="C34" s="30" t="inlineStr">
+      <c r="B34" s="29" t="n"/>
+      <c r="C34" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit Video:  Discussion. Play the video Return Visit: Prayer —1Jo 5:14. Stop the video at each pause, and ask the audience the questions that appear in the video.
 </t>
         </is>
       </c>
-      <c r="D34" s="29" t="n">
+      <c r="D34" s="31" t="n">
         <v>0.3173611111111111</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="32" t="inlineStr">
+      <c r="A35" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B35" s="15" t="n"/>
-      <c r="C35" s="33" t="inlineStr">
+      <c r="C35" s="35" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Use the sample conversation topic. (th study 15)
 </t>
         </is>
       </c>
-      <c r="D35" s="34" t="n">
+      <c r="D35" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="27" t="n"/>
-      <c r="B36" s="35" t="n"/>
-      <c r="C36" s="27" t="n"/>
-      <c r="D36" s="36" t="n"/>
+      <c r="A36" s="29" t="n"/>
+      <c r="B36" s="37" t="n"/>
+      <c r="C36" s="29" t="n"/>
+      <c r="D36" s="38" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="32" t="inlineStr">
+      <c r="A37" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B37" s="15" t="n"/>
-      <c r="C37" s="37" t="inlineStr">
+      <c r="C37" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 19)
 </t>
         </is>
       </c>
-      <c r="D37" s="34" t="n">
+      <c r="D37" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="27" t="n"/>
-      <c r="B38" s="35" t="n"/>
-      <c r="C38" s="27" t="n"/>
-      <c r="D38" s="36" t="n"/>
+      <c r="A38" s="29" t="n"/>
+      <c r="B38" s="37" t="n"/>
+      <c r="C38" s="29" t="n"/>
+      <c r="D38" s="38" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="15" t="n"/>
       <c r="B39" s="15" t="n"/>
       <c r="C39" s="15" t="inlineStr"/>
-      <c r="D39" s="25" t="n"/>
+      <c r="D39" s="27" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="21" t="inlineStr">
+      <c r="A40" s="40" t="inlineStr">
         <is>
           <t>Song 143</t>
         </is>
       </c>
       <c r="B40" s="15" t="n"/>
-      <c r="C40" s="38" t="inlineStr">
+      <c r="C40" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D40" s="25" t="n"/>
+      <c r="D40" s="27" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="26" t="inlineStr">
+      <c r="A41" s="28" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B41" s="27" t="n"/>
-      <c r="C41" s="28" t="inlineStr">
+      <c r="B41" s="29" t="n"/>
+      <c r="C41" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
 </t>
         </is>
       </c>
-      <c r="D41" s="29" t="n">
+      <c r="D41" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="26" t="inlineStr">
+      <c r="A42" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B42" s="27" t="n"/>
-      <c r="C42" s="28" t="inlineStr">
+      <c r="B42" s="29" t="n"/>
+      <c r="C42" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff section 2 review
 </t>
         </is>
       </c>
-      <c r="D42" s="29" t="n">
+      <c r="D42" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="26" t="inlineStr">
+      <c r="A43" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B43" s="27" t="n"/>
-      <c r="C43" s="28" t="inlineStr">
+      <c r="B43" s="29" t="n"/>
+      <c r="C43" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D43" s="29" t="n">
+      <c r="D43" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="21" t="inlineStr">
+      <c r="A44" s="40" t="inlineStr">
         <is>
           <t>Song 54</t>
         </is>
       </c>
       <c r="B44" s="15" t="n"/>
-      <c r="C44" s="22" t="inlineStr">
+      <c r="C44" s="42" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D44" s="25" t="n"/>
+      <c r="D44" s="27" t="n"/>
     </row>
     <row r="45" ht="21" customHeight="1">
-      <c r="A45" s="21" t="n"/>
+      <c r="A45" s="40" t="n"/>
       <c r="B45" s="15" t="n"/>
-      <c r="C45" s="22" t="n"/>
-      <c r="D45" s="25" t="n"/>
+      <c r="C45" s="42" t="n"/>
+      <c r="D45" s="27" t="n"/>
     </row>
     <row r="46" ht="21" customHeight="1">
       <c r="A46" s="17" t="inlineStr">
@@ -1357,13 +1372,13 @@
           <t>Song 96</t>
         </is>
       </c>
-      <c r="B47" s="15" t="n"/>
-      <c r="C47" s="22" t="inlineStr">
+      <c r="B47" s="22" t="n"/>
+      <c r="C47" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D47" s="23" t="inlineStr">
+      <c r="D47" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -1373,85 +1388,85 @@
       <c r="A48" s="15" t="n"/>
       <c r="B48" s="15" t="n"/>
       <c r="C48" s="15" t="n"/>
-      <c r="D48" s="23" t="n">
+      <c r="D48" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="15" t="n"/>
       <c r="B49" s="15" t="n"/>
-      <c r="C49" s="24" t="inlineStr">
+      <c r="C49" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D49" s="25" t="n"/>
+      <c r="D49" s="27" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="26" t="inlineStr">
+      <c r="A50" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B50" s="27" t="n"/>
-      <c r="C50" s="28" t="inlineStr">
+      <c r="B50" s="29" t="n"/>
+      <c r="C50" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D50" s="29" t="n">
+      <c r="D50" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="26" t="inlineStr">
+      <c r="A51" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B51" s="27" t="n"/>
-      <c r="C51" s="28" t="inlineStr">
+      <c r="B51" s="29" t="n"/>
+      <c r="C51" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“The Bible —A Book of Fact, Not Fiction”: 
 </t>
         </is>
       </c>
-      <c r="D51" s="29" t="n">
+      <c r="D51" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="26" t="inlineStr">
+      <c r="A52" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B52" s="27" t="n"/>
-      <c r="C52" s="30" t="inlineStr">
+      <c r="B52" s="29" t="n"/>
+      <c r="C52" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 3:1-3 —Why were women occasionally named in genealogical registers? (it-1 911 ¶3-4)
 </t>
         </is>
       </c>
-      <c r="D52" s="29" t="n">
+      <c r="D52" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="26" t="inlineStr">
+      <c r="A53" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B53" s="27" t="n"/>
-      <c r="C53" s="28" t="inlineStr">
+      <c r="B53" s="29" t="n"/>
+      <c r="C53" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 1:43-54 (th study 5)
 </t>
         </is>
       </c>
-      <c r="D53" s="29" t="n">
+      <c r="D53" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -1459,177 +1474,177 @@
       <c r="A54" s="15" t="n"/>
       <c r="B54" s="15" t="n"/>
       <c r="C54" s="15" t="inlineStr"/>
-      <c r="D54" s="25" t="n"/>
+      <c r="D54" s="27" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="15" t="n"/>
       <c r="B55" s="15" t="n"/>
-      <c r="C55" s="31" t="inlineStr">
+      <c r="C55" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D55" s="25" t="n"/>
+      <c r="D55" s="27" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="32" t="inlineStr">
+      <c r="A56" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B56" s="15" t="n"/>
-      <c r="C56" s="37" t="inlineStr">
+      <c r="C56" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a magazine to address a topic raised by the householder. (th study 4)
 </t>
         </is>
       </c>
-      <c r="D56" s="34" t="n">
+      <c r="D56" s="36" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="27" t="n"/>
-      <c r="B57" s="35" t="n"/>
-      <c r="C57" s="27" t="n"/>
-      <c r="D57" s="36" t="n"/>
+      <c r="A57" s="29" t="n"/>
+      <c r="B57" s="37" t="n"/>
+      <c r="C57" s="29" t="n"/>
+      <c r="D57" s="38" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="32" t="inlineStr">
+      <c r="A58" s="34" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B58" s="15" t="n"/>
-      <c r="C58" s="37" t="inlineStr">
+      <c r="C58" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 1)
 </t>
         </is>
       </c>
-      <c r="D58" s="34" t="n">
+      <c r="D58" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="27" t="n"/>
-      <c r="B59" s="35" t="n"/>
-      <c r="C59" s="27" t="n"/>
-      <c r="D59" s="36" t="n"/>
+      <c r="A59" s="29" t="n"/>
+      <c r="B59" s="37" t="n"/>
+      <c r="C59" s="29" t="n"/>
+      <c r="D59" s="38" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="32" t="inlineStr">
+      <c r="A60" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B60" s="15" t="n"/>
-      <c r="C60" s="37" t="inlineStr">
+      <c r="C60" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 point 7 and Some People Say (th study 8)
 </t>
         </is>
       </c>
-      <c r="D60" s="34" t="n">
+      <c r="D60" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="27" t="n"/>
-      <c r="B61" s="35" t="n"/>
-      <c r="C61" s="27" t="n"/>
-      <c r="D61" s="36" t="n"/>
+      <c r="A61" s="29" t="n"/>
+      <c r="B61" s="37" t="n"/>
+      <c r="C61" s="29" t="n"/>
+      <c r="D61" s="38" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="15" t="n"/>
       <c r="B62" s="15" t="n"/>
       <c r="C62" s="15" t="inlineStr"/>
-      <c r="D62" s="25" t="n"/>
+      <c r="D62" s="27" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="21" t="inlineStr">
+      <c r="A63" s="40" t="inlineStr">
         <is>
           <t>Song 98</t>
         </is>
       </c>
       <c r="B63" s="15" t="n"/>
-      <c r="C63" s="38" t="inlineStr">
+      <c r="C63" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D63" s="25" t="n"/>
+      <c r="D63" s="27" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="26" t="inlineStr">
+      <c r="A64" s="28" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B64" s="27" t="n"/>
-      <c r="C64" s="28" t="inlineStr">
+      <c r="B64" s="29" t="n"/>
+      <c r="C64" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Faith in God’s Word”:  Discussion and video.
 </t>
         </is>
       </c>
-      <c r="D64" s="29" t="n">
+      <c r="D64" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="26" t="inlineStr">
+      <c r="A65" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B65" s="27" t="n"/>
-      <c r="C65" s="28" t="inlineStr">
+      <c r="B65" s="29" t="n"/>
+      <c r="C65" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 34
 </t>
         </is>
       </c>
-      <c r="D65" s="29" t="n">
+      <c r="D65" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="26" t="inlineStr">
+      <c r="A66" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B66" s="27" t="n"/>
-      <c r="C66" s="28" t="inlineStr">
+      <c r="B66" s="29" t="n"/>
+      <c r="C66" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D66" s="29" t="n">
+      <c r="D66" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="21" t="inlineStr">
+      <c r="A67" s="40" t="inlineStr">
         <is>
           <t>Song 89</t>
         </is>
       </c>
       <c r="B67" s="15" t="n"/>
-      <c r="C67" s="22" t="inlineStr">
+      <c r="C67" s="42" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D67" s="25" t="n"/>
+      <c r="D67" s="27" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" s="21" t="n"/>
+      <c r="A68" s="40" t="n"/>
       <c r="B68" s="15" t="n"/>
-      <c r="C68" s="22" t="n"/>
-      <c r="D68" s="25" t="n"/>
+      <c r="C68" s="42" t="n"/>
+      <c r="D68" s="27" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="17" t="inlineStr">
@@ -1659,13 +1674,13 @@
           <t>Song 42</t>
         </is>
       </c>
-      <c r="B70" s="15" t="n"/>
-      <c r="C70" s="22" t="inlineStr">
+      <c r="B70" s="22" t="n"/>
+      <c r="C70" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D70" s="23" t="inlineStr">
+      <c r="D70" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -1675,85 +1690,85 @@
       <c r="A71" s="15" t="n"/>
       <c r="B71" s="15" t="n"/>
       <c r="C71" s="15" t="n"/>
-      <c r="D71" s="23" t="n">
+      <c r="D71" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="15" t="n"/>
       <c r="B72" s="15" t="n"/>
-      <c r="C72" s="24" t="inlineStr">
+      <c r="C72" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D72" s="25" t="n"/>
+      <c r="D72" s="27" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" s="26" t="inlineStr">
+      <c r="A73" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B73" s="27" t="n"/>
-      <c r="C73" s="28" t="inlineStr">
+      <c r="B73" s="29" t="n"/>
+      <c r="C73" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D73" s="29" t="n">
+      <c r="D73" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="26" t="inlineStr">
+      <c r="A74" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B74" s="27" t="n"/>
-      <c r="C74" s="28" t="inlineStr">
+      <c r="B74" s="29" t="n"/>
+      <c r="C74" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“What Do My Prayers Reveal About Me?”: 
 </t>
         </is>
       </c>
-      <c r="D74" s="29" t="n">
+      <c r="D74" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="26" t="inlineStr">
+      <c r="A75" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B75" s="27" t="n"/>
-      <c r="C75" s="30" t="inlineStr">
+      <c r="B75" s="29" t="n"/>
+      <c r="C75" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 5:10 —How can the victory over the Hagrites encourage us when we face seemingly insurmountable obstacles? (w05 10/1 9 ¶7)
 </t>
         </is>
       </c>
-      <c r="D75" s="29" t="n">
+      <c r="D75" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="26" t="inlineStr">
+      <c r="A76" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B76" s="27" t="n"/>
-      <c r="C76" s="28" t="inlineStr">
+      <c r="B76" s="29" t="n"/>
+      <c r="C76" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 6:61-81 (th study 2)
 </t>
         </is>
       </c>
-      <c r="D76" s="29" t="n">
+      <c r="D76" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -1761,192 +1776,192 @@
       <c r="A77" s="15" t="n"/>
       <c r="B77" s="15" t="n"/>
       <c r="C77" s="15" t="inlineStr"/>
-      <c r="D77" s="25" t="n"/>
+      <c r="D77" s="27" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="15" t="n"/>
       <c r="B78" s="15" t="n"/>
-      <c r="C78" s="31" t="inlineStr">
+      <c r="C78" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D78" s="25" t="n"/>
+      <c r="D78" s="27" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" s="32" t="inlineStr">
+      <c r="A79" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B79" s="15" t="n"/>
-      <c r="C79" s="37" t="inlineStr">
+      <c r="C79" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Use the sample conversation topic. Respond to a common objection. (th study 3)
 </t>
         </is>
       </c>
-      <c r="D79" s="34" t="n">
+      <c r="D79" s="36" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="27" t="n"/>
-      <c r="B80" s="35" t="n"/>
-      <c r="C80" s="27" t="n"/>
-      <c r="D80" s="36" t="n"/>
+      <c r="A80" s="29" t="n"/>
+      <c r="B80" s="37" t="n"/>
+      <c r="C80" s="29" t="n"/>
+      <c r="D80" s="38" t="n"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="32" t="inlineStr">
+      <c r="A81" s="34" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B81" s="15" t="n"/>
-      <c r="C81" s="37" t="inlineStr">
+      <c r="C81" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Why Study the Bible? (th study 14)
 </t>
         </is>
       </c>
-      <c r="D81" s="34" t="n">
+      <c r="D81" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="27" t="n"/>
-      <c r="B82" s="35" t="n"/>
-      <c r="C82" s="27" t="n"/>
-      <c r="D82" s="36" t="n"/>
+      <c r="A82" s="29" t="n"/>
+      <c r="B82" s="37" t="n"/>
+      <c r="C82" s="29" t="n"/>
+      <c r="D82" s="38" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" s="32" t="inlineStr">
+      <c r="A83" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B83" s="15" t="n"/>
-      <c r="C83" s="37" t="inlineStr">
+      <c r="C83" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 summary, review, and goal (th study 9)
 </t>
         </is>
       </c>
-      <c r="D83" s="34" t="n">
+      <c r="D83" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="27" t="n"/>
-      <c r="B84" s="35" t="n"/>
-      <c r="C84" s="27" t="n"/>
-      <c r="D84" s="36" t="n"/>
+      <c r="A84" s="29" t="n"/>
+      <c r="B84" s="37" t="n"/>
+      <c r="C84" s="29" t="n"/>
+      <c r="D84" s="38" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="15" t="n"/>
       <c r="B85" s="15" t="n"/>
       <c r="C85" s="15" t="inlineStr"/>
-      <c r="D85" s="25" t="n"/>
+      <c r="D85" s="27" t="n"/>
     </row>
     <row r="86">
-      <c r="A86" s="21" t="inlineStr">
+      <c r="A86" s="40" t="inlineStr">
         <is>
           <t>Song 127</t>
         </is>
       </c>
       <c r="B86" s="15" t="n"/>
-      <c r="C86" s="38" t="inlineStr">
+      <c r="C86" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D86" s="25" t="n"/>
+      <c r="D86" s="27" t="n"/>
     </row>
     <row r="87">
-      <c r="A87" s="26" t="inlineStr">
+      <c r="A87" s="28" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B87" s="27" t="n"/>
-      <c r="C87" s="30" t="inlineStr">
+      <c r="B87" s="29" t="n"/>
+      <c r="C87" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">“Prepare Now for a Medical Emergency”:  Discussion and video. To be handled by an elder. Allow time for several comments after the video.
 </t>
         </is>
       </c>
-      <c r="D87" s="29" t="n">
+      <c r="D87" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="26" t="inlineStr">
+      <c r="A88" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B88" s="27" t="n"/>
-      <c r="C88" s="28" t="inlineStr">
+      <c r="B88" s="29" t="n"/>
+      <c r="C88" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 35
 </t>
         </is>
       </c>
-      <c r="D88" s="29" t="n">
+      <c r="D88" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="26" t="inlineStr">
+      <c r="A89" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B89" s="27" t="n"/>
-      <c r="C89" s="28" t="inlineStr">
+      <c r="B89" s="29" t="n"/>
+      <c r="C89" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D89" s="29" t="n">
+      <c r="D89" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="39" t="inlineStr">
+      <c r="A90" s="43" t="inlineStr">
         <is>
           <t>Song 88</t>
         </is>
       </c>
-      <c r="B90" s="27" t="n"/>
-      <c r="C90" s="40" t="inlineStr">
+      <c r="B90" s="29" t="n"/>
+      <c r="C90" s="44" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D90" s="36" t="n"/>
+      <c r="D90" s="38" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="15" t="n"/>
       <c r="B91" s="15" t="n"/>
-      <c r="C91" s="41" t="n"/>
+      <c r="C91" s="45" t="n"/>
       <c r="D91" s="15" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="15" t="n"/>
       <c r="B92" s="15" t="n"/>
-      <c r="C92" s="41" t="n"/>
+      <c r="C92" s="45" t="n"/>
       <c r="D92" s="15" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="15" t="n"/>
-      <c r="B93" s="42" t="inlineStr">
+      <c r="B93" s="46" t="inlineStr">
         <is>
           <t>Life and Ministry Meeting Workbook, February 2023</t>
         </is>
       </c>
-      <c r="C93" s="43" t="n"/>
+      <c r="C93" s="47" t="n"/>
       <c r="D93" s="15" t="n"/>
     </row>
     <row r="94">
@@ -1955,7 +1970,7 @@
           <t>Week 1</t>
         </is>
       </c>
-      <c r="B94" s="44" t="inlineStr">
+      <c r="B94" s="48" t="inlineStr">
         <is>
           <t>January 30 - February 5</t>
         </is>
@@ -1977,13 +1992,13 @@
           <t>Song 84</t>
         </is>
       </c>
-      <c r="B95" s="15" t="n"/>
-      <c r="C95" s="22" t="inlineStr">
+      <c r="B95" s="22" t="n"/>
+      <c r="C95" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D95" s="23" t="inlineStr">
+      <c r="D95" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -1993,85 +2008,85 @@
       <c r="A96" s="15" t="n"/>
       <c r="B96" s="15" t="n"/>
       <c r="C96" s="15" t="n"/>
-      <c r="D96" s="23" t="n">
+      <c r="D96" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="15" t="n"/>
       <c r="B97" s="15" t="n"/>
-      <c r="C97" s="24" t="inlineStr">
+      <c r="C97" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D97" s="25" t="n"/>
+      <c r="D97" s="27" t="n"/>
     </row>
     <row r="98">
-      <c r="A98" s="26" t="inlineStr">
+      <c r="A98" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B98" s="27" t="n"/>
-      <c r="C98" s="28" t="inlineStr">
+      <c r="B98" s="29" t="n"/>
+      <c r="C98" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D98" s="29" t="n">
+      <c r="D98" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="26" t="inlineStr">
+      <c r="A99" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B99" s="27" t="n"/>
-      <c r="C99" s="28" t="inlineStr">
+      <c r="B99" s="29" t="n"/>
+      <c r="C99" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“You Can Fulfill Challenging Assignments With Jehovah’s Help”: 
 </t>
         </is>
       </c>
-      <c r="D99" s="29" t="n">
+      <c r="D99" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="26" t="inlineStr">
+      <c r="A100" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B100" s="27" t="n"/>
-      <c r="C100" s="30" t="inlineStr">
+      <c r="B100" s="29" t="n"/>
+      <c r="C100" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 9:33 —How does this verse help us to appreciate the importance of music in true worship? (w10 12/15 21 ¶6)
 </t>
         </is>
       </c>
-      <c r="D100" s="29" t="n">
+      <c r="D100" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="26" t="inlineStr">
+      <c r="A101" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B101" s="27" t="n"/>
-      <c r="C101" s="28" t="inlineStr">
+      <c r="B101" s="29" t="n"/>
+      <c r="C101" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 7:1-13 (th study 10)
 </t>
         </is>
       </c>
-      <c r="D101" s="29" t="n">
+      <c r="D101" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -2079,177 +2094,177 @@
       <c r="A102" s="15" t="n"/>
       <c r="B102" s="15" t="n"/>
       <c r="C102" s="15" t="inlineStr"/>
-      <c r="D102" s="25" t="n"/>
+      <c r="D102" s="27" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="15" t="n"/>
       <c r="B103" s="15" t="n"/>
-      <c r="C103" s="31" t="inlineStr">
+      <c r="C103" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D103" s="25" t="n"/>
+      <c r="D103" s="27" t="n"/>
     </row>
     <row r="104">
-      <c r="A104" s="32" t="inlineStr">
+      <c r="A104" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B104" s="15" t="n"/>
-      <c r="C104" s="37" t="inlineStr">
+      <c r="C104" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Leave a jw.org contact card. (th study 16)
 </t>
         </is>
       </c>
-      <c r="D104" s="34" t="n">
+      <c r="D104" s="36" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="27" t="n"/>
-      <c r="B105" s="35" t="n"/>
-      <c r="C105" s="27" t="n"/>
-      <c r="D105" s="36" t="n"/>
+      <c r="A105" s="29" t="n"/>
+      <c r="B105" s="37" t="n"/>
+      <c r="C105" s="29" t="n"/>
+      <c r="D105" s="38" t="n"/>
     </row>
     <row r="106">
-      <c r="A106" s="32" t="inlineStr">
+      <c r="A106" s="34" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B106" s="15" t="n"/>
-      <c r="C106" s="37" t="inlineStr">
+      <c r="C106" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 20)
 </t>
         </is>
       </c>
-      <c r="D106" s="34" t="n">
+      <c r="D106" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="27" t="n"/>
-      <c r="B107" s="35" t="n"/>
-      <c r="C107" s="27" t="n"/>
-      <c r="D107" s="36" t="n"/>
+      <c r="A107" s="29" t="n"/>
+      <c r="B107" s="37" t="n"/>
+      <c r="C107" s="29" t="n"/>
+      <c r="D107" s="38" t="n"/>
     </row>
     <row r="108">
-      <c r="A108" s="32" t="inlineStr">
+      <c r="A108" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B108" s="15" t="n"/>
-      <c r="C108" s="37" t="inlineStr">
+      <c r="C108" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w21.06 3-4 ¶3-8 —Theme: Help Your Bible Student to Apply What He Is Learning. (th study 13)
 </t>
         </is>
       </c>
-      <c r="D108" s="34" t="n">
+      <c r="D108" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="27" t="n"/>
-      <c r="B109" s="35" t="n"/>
-      <c r="C109" s="27" t="n"/>
-      <c r="D109" s="36" t="n"/>
+      <c r="A109" s="29" t="n"/>
+      <c r="B109" s="37" t="n"/>
+      <c r="C109" s="29" t="n"/>
+      <c r="D109" s="38" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="15" t="n"/>
       <c r="B110" s="15" t="n"/>
       <c r="C110" s="15" t="inlineStr"/>
-      <c r="D110" s="25" t="n"/>
+      <c r="D110" s="27" t="n"/>
     </row>
     <row r="111">
-      <c r="A111" s="21" t="inlineStr">
+      <c r="A111" s="40" t="inlineStr">
         <is>
           <t>Song 38</t>
         </is>
       </c>
       <c r="B111" s="15" t="n"/>
-      <c r="C111" s="38" t="inlineStr">
+      <c r="C111" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D111" s="25" t="n"/>
+      <c r="D111" s="27" t="n"/>
     </row>
     <row r="112">
-      <c r="A112" s="26" t="inlineStr">
+      <c r="A112" s="28" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B112" s="27" t="n"/>
-      <c r="C112" s="28" t="inlineStr">
+      <c r="B112" s="29" t="n"/>
+      <c r="C112" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Jehovah Helps Us Through Our Trials”:  Discussion and video.
 </t>
         </is>
       </c>
-      <c r="D112" s="29" t="n">
+      <c r="D112" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="26" t="inlineStr">
+      <c r="A113" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B113" s="27" t="n"/>
-      <c r="C113" s="28" t="inlineStr">
+      <c r="B113" s="29" t="n"/>
+      <c r="C113" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 36
 </t>
         </is>
       </c>
-      <c r="D113" s="29" t="n">
+      <c r="D113" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="26" t="inlineStr">
+      <c r="A114" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B114" s="27" t="n"/>
-      <c r="C114" s="28" t="inlineStr">
+      <c r="B114" s="29" t="n"/>
+      <c r="C114" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D114" s="29" t="n">
+      <c r="D114" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="21" t="inlineStr">
+      <c r="A115" s="40" t="inlineStr">
         <is>
           <t>Song 31</t>
         </is>
       </c>
       <c r="B115" s="15" t="n"/>
-      <c r="C115" s="22" t="inlineStr">
+      <c r="C115" s="42" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D115" s="25" t="n"/>
+      <c r="D115" s="27" t="n"/>
     </row>
     <row r="116">
-      <c r="A116" s="21" t="n"/>
+      <c r="A116" s="40" t="n"/>
       <c r="B116" s="15" t="n"/>
-      <c r="C116" s="22" t="n"/>
-      <c r="D116" s="25" t="n"/>
+      <c r="C116" s="42" t="n"/>
+      <c r="D116" s="27" t="n"/>
     </row>
     <row r="117">
       <c r="A117" s="17" t="inlineStr">
@@ -2279,13 +2294,13 @@
           <t>Song 94</t>
         </is>
       </c>
-      <c r="B118" s="15" t="n"/>
-      <c r="C118" s="22" t="inlineStr">
+      <c r="B118" s="22" t="n"/>
+      <c r="C118" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D118" s="23" t="inlineStr">
+      <c r="D118" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -2295,85 +2310,85 @@
       <c r="A119" s="15" t="n"/>
       <c r="B119" s="15" t="n"/>
       <c r="C119" s="15" t="n"/>
-      <c r="D119" s="23" t="n">
+      <c r="D119" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="15" t="n"/>
       <c r="B120" s="15" t="n"/>
-      <c r="C120" s="24" t="inlineStr">
+      <c r="C120" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D120" s="25" t="n"/>
+      <c r="D120" s="27" t="n"/>
     </row>
     <row r="121">
-      <c r="A121" s="26" t="inlineStr">
+      <c r="A121" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B121" s="27" t="n"/>
-      <c r="C121" s="28" t="inlineStr">
+      <c r="B121" s="29" t="n"/>
+      <c r="C121" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D121" s="29" t="n">
+      <c r="D121" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="26" t="inlineStr">
+      <c r="A122" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B122" s="27" t="n"/>
-      <c r="C122" s="28" t="inlineStr">
+      <c r="B122" s="29" t="n"/>
+      <c r="C122" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Desire to Do God’s Will”: 
 </t>
         </is>
       </c>
-      <c r="D122" s="29" t="n">
+      <c r="D122" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="26" t="inlineStr">
+      <c r="A123" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B123" s="27" t="n"/>
-      <c r="C123" s="30" t="inlineStr">
+      <c r="B123" s="29" t="n"/>
+      <c r="C123" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 12:33 —What good example did the 50,000 men of Zebulun set? (it-1 1058 ¶5-6)
 </t>
         </is>
       </c>
-      <c r="D123" s="29" t="n">
+      <c r="D123" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="26" t="inlineStr">
+      <c r="A124" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B124" s="27" t="n"/>
-      <c r="C124" s="28" t="inlineStr">
+      <c r="B124" s="29" t="n"/>
+      <c r="C124" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 11:26-47 (th study 5)
 </t>
         </is>
       </c>
-      <c r="D124" s="29" t="n">
+      <c r="D124" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -2381,194 +2396,194 @@
       <c r="A125" s="15" t="n"/>
       <c r="B125" s="15" t="n"/>
       <c r="C125" s="15" t="inlineStr"/>
-      <c r="D125" s="25" t="n"/>
+      <c r="D125" s="27" t="n"/>
     </row>
     <row r="126">
       <c r="A126" s="15" t="n"/>
       <c r="B126" s="15" t="n"/>
-      <c r="C126" s="31" t="inlineStr">
+      <c r="C126" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D126" s="25" t="n"/>
+      <c r="D126" s="27" t="n"/>
     </row>
     <row r="127">
-      <c r="A127" s="32" t="inlineStr">
+      <c r="A127" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B127" s="15" t="n"/>
-      <c r="C127" s="37" t="inlineStr">
+      <c r="C127" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a Bible study. (th study 12)
 </t>
         </is>
       </c>
-      <c r="D127" s="34" t="n">
+      <c r="D127" s="36" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="27" t="n"/>
-      <c r="B128" s="35" t="n"/>
-      <c r="C128" s="27" t="n"/>
-      <c r="D128" s="36" t="n"/>
+      <c r="A128" s="29" t="n"/>
+      <c r="B128" s="37" t="n"/>
+      <c r="C128" s="29" t="n"/>
+      <c r="D128" s="38" t="n"/>
     </row>
     <row r="129">
-      <c r="A129" s="32" t="inlineStr">
+      <c r="A129" s="34" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B129" s="15" t="n"/>
-      <c r="C129" s="37" t="inlineStr">
+      <c r="C129" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video What Happens at a Bible Study? (th study 6)
 </t>
         </is>
       </c>
-      <c r="D129" s="34" t="n">
+      <c r="D129" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="27" t="n"/>
-      <c r="B130" s="35" t="n"/>
-      <c r="C130" s="27" t="n"/>
-      <c r="D130" s="36" t="n"/>
+      <c r="A130" s="29" t="n"/>
+      <c r="B130" s="37" t="n"/>
+      <c r="C130" s="29" t="n"/>
+      <c r="D130" s="38" t="n"/>
     </row>
     <row r="131">
-      <c r="A131" s="32" t="inlineStr">
+      <c r="A131" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B131" s="15" t="n"/>
-      <c r="C131" s="33" t="inlineStr">
+      <c r="C131" s="35" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 09 intro and points 1-3 (th study 18)
 </t>
         </is>
       </c>
-      <c r="D131" s="34" t="n">
+      <c r="D131" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="27" t="n"/>
-      <c r="B132" s="35" t="n"/>
-      <c r="C132" s="27" t="n"/>
-      <c r="D132" s="36" t="n"/>
+      <c r="A132" s="29" t="n"/>
+      <c r="B132" s="37" t="n"/>
+      <c r="C132" s="29" t="n"/>
+      <c r="D132" s="38" t="n"/>
     </row>
     <row r="133">
       <c r="A133" s="15" t="n"/>
       <c r="B133" s="15" t="n"/>
       <c r="C133" s="15" t="inlineStr"/>
-      <c r="D133" s="25" t="n"/>
+      <c r="D133" s="27" t="n"/>
     </row>
     <row r="134">
-      <c r="A134" s="21" t="inlineStr">
+      <c r="A134" s="40" t="inlineStr">
         <is>
           <t>Song 97</t>
         </is>
       </c>
       <c r="B134" s="15" t="n"/>
-      <c r="C134" s="38" t="inlineStr">
+      <c r="C134" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D134" s="25" t="n"/>
+      <c r="D134" s="27" t="n"/>
     </row>
     <row r="135">
-      <c r="A135" s="26" t="inlineStr">
+      <c r="A135" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B135" s="27" t="n"/>
-      <c r="C135" s="28" t="inlineStr">
+      <c r="B135" s="29" t="n"/>
+      <c r="C135" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Search for God’s Thinking”:  Discussion and video.
 </t>
         </is>
       </c>
-      <c r="D135" s="29" t="n">
+      <c r="D135" s="31" t="n">
         <v>0.33125</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="26" t="inlineStr">
+      <c r="A136" s="28" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B136" s="27" t="n"/>
-      <c r="C136" s="28" t="inlineStr">
+      <c r="B136" s="29" t="n"/>
+      <c r="C136" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Set Goals for the Memorial Season”:  Discussion.
 </t>
         </is>
       </c>
-      <c r="D136" s="29" t="n">
+      <c r="D136" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="26" t="inlineStr">
+      <c r="A137" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B137" s="27" t="n"/>
-      <c r="C137" s="28" t="inlineStr">
+      <c r="B137" s="29" t="n"/>
+      <c r="C137" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 points 1-5
 </t>
         </is>
       </c>
-      <c r="D137" s="29" t="n">
+      <c r="D137" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="26" t="inlineStr">
+      <c r="A138" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B138" s="27" t="n"/>
-      <c r="C138" s="28" t="inlineStr">
+      <c r="B138" s="29" t="n"/>
+      <c r="C138" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D138" s="29" t="n">
+      <c r="D138" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="21" t="inlineStr">
+      <c r="A139" s="40" t="inlineStr">
         <is>
           <t>Song 91</t>
         </is>
       </c>
       <c r="B139" s="15" t="n"/>
-      <c r="C139" s="22" t="inlineStr">
+      <c r="C139" s="42" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D139" s="25" t="n"/>
+      <c r="D139" s="27" t="n"/>
     </row>
     <row r="140">
-      <c r="A140" s="21" t="n"/>
+      <c r="A140" s="40" t="n"/>
       <c r="B140" s="15" t="n"/>
-      <c r="C140" s="22" t="n"/>
-      <c r="D140" s="25" t="n"/>
+      <c r="C140" s="42" t="n"/>
+      <c r="D140" s="27" t="n"/>
     </row>
     <row r="141">
       <c r="A141" s="17" t="inlineStr">
@@ -2598,13 +2613,13 @@
           <t>Song 123</t>
         </is>
       </c>
-      <c r="B142" s="15" t="n"/>
-      <c r="C142" s="22" t="inlineStr">
+      <c r="B142" s="22" t="n"/>
+      <c r="C142" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D142" s="23" t="inlineStr">
+      <c r="D142" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -2614,85 +2629,85 @@
       <c r="A143" s="15" t="n"/>
       <c r="B143" s="15" t="n"/>
       <c r="C143" s="15" t="n"/>
-      <c r="D143" s="23" t="n">
+      <c r="D143" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="15" t="n"/>
       <c r="B144" s="15" t="n"/>
-      <c r="C144" s="24" t="inlineStr">
+      <c r="C144" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D144" s="25" t="n"/>
+      <c r="D144" s="27" t="n"/>
     </row>
     <row r="145">
-      <c r="A145" s="26" t="inlineStr">
+      <c r="A145" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B145" s="27" t="n"/>
-      <c r="C145" s="28" t="inlineStr">
+      <c r="B145" s="29" t="n"/>
+      <c r="C145" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D145" s="29" t="n">
+      <c r="D145" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="26" t="inlineStr">
+      <c r="A146" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B146" s="27" t="n"/>
-      <c r="C146" s="28" t="inlineStr">
+      <c r="B146" s="29" t="n"/>
+      <c r="C146" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Following Direction Leads to Success”: 
 </t>
         </is>
       </c>
-      <c r="D146" s="29" t="n">
+      <c r="D146" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="26" t="inlineStr">
+      <c r="A147" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B147" s="27" t="n"/>
-      <c r="C147" s="30" t="inlineStr">
+      <c r="B147" s="29" t="n"/>
+      <c r="C147" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 16:31 —Why could the Levites sing: “Jehovah has become King!”? (w14 1/15 10 ¶14)
 </t>
         </is>
       </c>
-      <c r="D147" s="29" t="n">
+      <c r="D147" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="26" t="inlineStr">
+      <c r="A148" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B148" s="27" t="n"/>
-      <c r="C148" s="28" t="inlineStr">
+      <c r="B148" s="29" t="n"/>
+      <c r="C148" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 13:1-14 (th study 11)
 </t>
         </is>
       </c>
-      <c r="D148" s="29" t="n">
+      <c r="D148" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -2700,194 +2715,194 @@
       <c r="A149" s="15" t="n"/>
       <c r="B149" s="15" t="n"/>
       <c r="C149" s="15" t="inlineStr"/>
-      <c r="D149" s="25" t="n"/>
+      <c r="D149" s="27" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="15" t="n"/>
       <c r="B150" s="15" t="n"/>
-      <c r="C150" s="31" t="inlineStr">
+      <c r="C150" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D150" s="25" t="n"/>
+      <c r="D150" s="27" t="n"/>
     </row>
     <row r="151">
-      <c r="A151" s="32" t="inlineStr">
+      <c r="A151" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B151" s="15" t="n"/>
-      <c r="C151" s="37" t="inlineStr">
+      <c r="C151" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Respond to a common objection. (th study 18)
 </t>
         </is>
       </c>
-      <c r="D151" s="34" t="n">
+      <c r="D151" s="36" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="27" t="n"/>
-      <c r="B152" s="35" t="n"/>
-      <c r="C152" s="27" t="n"/>
-      <c r="D152" s="36" t="n"/>
+      <c r="A152" s="29" t="n"/>
+      <c r="B152" s="37" t="n"/>
+      <c r="C152" s="29" t="n"/>
+      <c r="D152" s="38" t="n"/>
     </row>
     <row r="153">
-      <c r="A153" s="32" t="inlineStr">
+      <c r="A153" s="34" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B153" s="15" t="n"/>
-      <c r="C153" s="37" t="inlineStr">
+      <c r="C153" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 7)
 </t>
         </is>
       </c>
-      <c r="D153" s="34" t="n">
+      <c r="D153" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="27" t="n"/>
-      <c r="B154" s="35" t="n"/>
-      <c r="C154" s="27" t="n"/>
-      <c r="D154" s="36" t="n"/>
+      <c r="A154" s="29" t="n"/>
+      <c r="B154" s="37" t="n"/>
+      <c r="C154" s="29" t="n"/>
+      <c r="D154" s="38" t="n"/>
     </row>
     <row r="155">
-      <c r="A155" s="32" t="inlineStr">
+      <c r="A155" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B155" s="15" t="n"/>
-      <c r="C155" s="37" t="inlineStr">
+      <c r="C155" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w16.01 13-14 ¶7-10 —Theme: “The Love the Christ Has Compels Us.” —2Co 5:14. (th study 8)
 </t>
         </is>
       </c>
-      <c r="D155" s="34" t="n">
+      <c r="D155" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="27" t="n"/>
-      <c r="B156" s="35" t="n"/>
-      <c r="C156" s="27" t="n"/>
-      <c r="D156" s="36" t="n"/>
+      <c r="A156" s="29" t="n"/>
+      <c r="B156" s="37" t="n"/>
+      <c r="C156" s="29" t="n"/>
+      <c r="D156" s="38" t="n"/>
     </row>
     <row r="157">
       <c r="A157" s="15" t="n"/>
       <c r="B157" s="15" t="n"/>
       <c r="C157" s="15" t="inlineStr"/>
-      <c r="D157" s="25" t="n"/>
+      <c r="D157" s="27" t="n"/>
     </row>
     <row r="158">
-      <c r="A158" s="21" t="inlineStr">
+      <c r="A158" s="40" t="inlineStr">
         <is>
           <t>Song 86</t>
         </is>
       </c>
       <c r="B158" s="15" t="n"/>
-      <c r="C158" s="38" t="inlineStr">
+      <c r="C158" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D158" s="25" t="n"/>
+      <c r="D158" s="27" t="n"/>
     </row>
     <row r="159">
-      <c r="A159" s="26" t="inlineStr">
+      <c r="A159" s="28" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B159" s="27" t="n"/>
-      <c r="C159" s="30" t="inlineStr">
+      <c r="B159" s="29" t="n"/>
+      <c r="C159" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Become Jehovah’s Friend —Pay Attention at the Meetings:  Discussion. Play the video. Then, if possible, ask selected children: Why should we pay attention at meetings? What can help you to do so?
 </t>
         </is>
       </c>
-      <c r="D159" s="29" t="n">
+      <c r="D159" s="31" t="n">
         <v>0.3277777777777778</v>
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="26" t="inlineStr">
+      <c r="A160" s="28" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B160" s="27" t="n"/>
-      <c r="C160" s="28" t="inlineStr">
+      <c r="B160" s="29" t="n"/>
+      <c r="C160" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
 </t>
         </is>
       </c>
-      <c r="D160" s="29" t="n">
+      <c r="D160" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="26" t="inlineStr">
+      <c r="A161" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B161" s="27" t="n"/>
-      <c r="C161" s="30" t="inlineStr">
+      <c r="B161" s="29" t="n"/>
+      <c r="C161" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 point 6 and summary, review, and goal
 </t>
         </is>
       </c>
-      <c r="D161" s="29" t="n">
+      <c r="D161" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="26" t="inlineStr">
+      <c r="A162" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B162" s="27" t="n"/>
-      <c r="C162" s="28" t="inlineStr">
+      <c r="B162" s="29" t="n"/>
+      <c r="C162" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D162" s="29" t="n">
+      <c r="D162" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="21" t="inlineStr">
+      <c r="A163" s="40" t="inlineStr">
         <is>
           <t>Song 21</t>
         </is>
       </c>
       <c r="B163" s="15" t="n"/>
-      <c r="C163" s="22" t="inlineStr">
+      <c r="C163" s="42" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D163" s="25" t="n"/>
+      <c r="D163" s="27" t="n"/>
     </row>
     <row r="164">
-      <c r="A164" s="21" t="n"/>
+      <c r="A164" s="40" t="n"/>
       <c r="B164" s="15" t="n"/>
-      <c r="C164" s="22" t="n"/>
-      <c r="D164" s="25" t="n"/>
+      <c r="C164" s="42" t="n"/>
+      <c r="D164" s="27" t="n"/>
     </row>
     <row r="165">
       <c r="A165" s="17" t="inlineStr">
@@ -2917,13 +2932,13 @@
           <t>Song 110</t>
         </is>
       </c>
-      <c r="B166" s="15" t="n"/>
-      <c r="C166" s="22" t="inlineStr">
+      <c r="B166" s="22" t="n"/>
+      <c r="C166" s="23" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D166" s="23" t="inlineStr">
+      <c r="D166" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
@@ -2933,85 +2948,85 @@
       <c r="A167" s="15" t="n"/>
       <c r="B167" s="15" t="n"/>
       <c r="C167" s="15" t="n"/>
-      <c r="D167" s="23" t="n">
+      <c r="D167" s="25" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="15" t="n"/>
       <c r="B168" s="15" t="n"/>
-      <c r="C168" s="24" t="inlineStr">
+      <c r="C168" s="26" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D168" s="25" t="n"/>
+      <c r="D168" s="27" t="n"/>
     </row>
     <row r="169">
-      <c r="A169" s="26" t="inlineStr">
+      <c r="A169" s="28" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B169" s="27" t="n"/>
-      <c r="C169" s="28" t="inlineStr">
+      <c r="B169" s="29" t="n"/>
+      <c r="C169" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
  </t>
         </is>
       </c>
-      <c r="D169" s="29" t="n">
+      <c r="D169" s="31" t="n">
         <v>0.2965277777777778</v>
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="26" t="inlineStr">
+      <c r="A170" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B170" s="27" t="n"/>
-      <c r="C170" s="28" t="inlineStr">
+      <c r="B170" s="29" t="n"/>
+      <c r="C170" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">“Maintain Your Joy Despite Disappointments”: 
 </t>
         </is>
       </c>
-      <c r="D170" s="29" t="n">
+      <c r="D170" s="31" t="n">
         <v>0.3034722222222222</v>
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="26" t="inlineStr">
+      <c r="A171" s="28" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B171" s="27" t="n"/>
-      <c r="C171" s="30" t="inlineStr">
+      <c r="B171" s="29" t="n"/>
+      <c r="C171" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems:  1Ch 17:16-18 —Like David, of what can we be confident? (w20.02 12, box)
 </t>
         </is>
       </c>
-      <c r="D171" s="29" t="n">
+      <c r="D171" s="31" t="n">
         <v>0.3104166666666667</v>
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="26" t="inlineStr">
+      <c r="A172" s="28" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B172" s="27" t="n"/>
-      <c r="C172" s="28" t="inlineStr">
+      <c r="B172" s="29" t="n"/>
+      <c r="C172" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 18:1-17 (th study 2)
 </t>
         </is>
       </c>
-      <c r="D172" s="29" t="n">
+      <c r="D172" s="31" t="n">
         <v>0.3138888888888889</v>
       </c>
     </row>
@@ -3019,155 +3034,155 @@
       <c r="A173" s="15" t="n"/>
       <c r="B173" s="15" t="n"/>
       <c r="C173" s="15" t="inlineStr"/>
-      <c r="D173" s="25" t="n"/>
+      <c r="D173" s="27" t="n"/>
     </row>
     <row r="174">
       <c r="A174" s="15" t="n"/>
       <c r="B174" s="15" t="n"/>
-      <c r="C174" s="31" t="inlineStr">
+      <c r="C174" s="33" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D174" s="25" t="n"/>
+      <c r="D174" s="27" t="n"/>
     </row>
     <row r="175">
-      <c r="A175" s="32" t="inlineStr">
+      <c r="A175" s="34" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
       <c r="B175" s="15" t="n"/>
-      <c r="C175" s="37" t="inlineStr">
+      <c r="C175" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Jehovah’s Witnesses —Who Are We? (th study 17)
 </t>
         </is>
       </c>
-      <c r="D175" s="34" t="n">
+      <c r="D175" s="36" t="n">
         <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="27" t="n"/>
-      <c r="B176" s="35" t="n"/>
-      <c r="C176" s="27" t="n"/>
-      <c r="D176" s="36" t="n"/>
+      <c r="A176" s="29" t="n"/>
+      <c r="B176" s="37" t="n"/>
+      <c r="C176" s="29" t="n"/>
+      <c r="D176" s="38" t="n"/>
     </row>
     <row r="177">
-      <c r="A177" s="32" t="inlineStr">
+      <c r="A177" s="34" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
       <c r="B177" s="15" t="n"/>
-      <c r="C177" s="37" t="inlineStr">
+      <c r="C177" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 3)
 </t>
         </is>
       </c>
-      <c r="D177" s="34" t="n">
+      <c r="D177" s="36" t="n">
         <v>0.3201388888888889</v>
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="27" t="n"/>
-      <c r="B178" s="35" t="n"/>
-      <c r="C178" s="27" t="n"/>
-      <c r="D178" s="36" t="n"/>
+      <c r="A178" s="29" t="n"/>
+      <c r="B178" s="37" t="n"/>
+      <c r="C178" s="29" t="n"/>
+      <c r="D178" s="38" t="n"/>
     </row>
     <row r="179">
-      <c r="A179" s="32" t="inlineStr">
+      <c r="A179" s="34" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
       <c r="B179" s="15" t="n"/>
-      <c r="C179" s="33" t="inlineStr">
+      <c r="C179" s="35" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 09 point 4 (th study 9)
 </t>
         </is>
       </c>
-      <c r="D179" s="34" t="n">
+      <c r="D179" s="36" t="n">
         <v>0.3243055555555556</v>
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="27" t="n"/>
-      <c r="B180" s="35" t="n"/>
-      <c r="C180" s="27" t="n"/>
-      <c r="D180" s="36" t="n"/>
+      <c r="A180" s="29" t="n"/>
+      <c r="B180" s="37" t="n"/>
+      <c r="C180" s="29" t="n"/>
+      <c r="D180" s="38" t="n"/>
     </row>
     <row r="181">
       <c r="A181" s="15" t="n"/>
       <c r="B181" s="15" t="n"/>
       <c r="C181" s="15" t="inlineStr"/>
-      <c r="D181" s="25" t="n"/>
+      <c r="D181" s="27" t="n"/>
     </row>
     <row r="182">
-      <c r="A182" s="21" t="inlineStr">
+      <c r="A182" s="40" t="inlineStr">
         <is>
           <t>Song 64</t>
         </is>
       </c>
       <c r="B182" s="15" t="n"/>
-      <c r="C182" s="38" t="inlineStr">
+      <c r="C182" s="41" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D182" s="25" t="n"/>
+      <c r="D182" s="27" t="n"/>
     </row>
     <row r="183">
-      <c r="A183" s="26" t="inlineStr">
+      <c r="A183" s="28" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B183" s="27" t="n"/>
-      <c r="C183" s="30" t="inlineStr">
+      <c r="B183" s="29" t="n"/>
+      <c r="C183" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Annual Service Report:  Discussion. After reading the announcement from the branch office regarding the annual service report, invite the audience to highlight other positive aspects of the 2022 Service Year Report of Jehovah’s Witnesses Worldwide. Interview publishers, selected in advance, who had encouraging experiences in the ministry during the past year.
 </t>
         </is>
       </c>
-      <c r="D183" s="29" t="n">
+      <c r="D183" s="31" t="n">
         <v>0.3381944444444445</v>
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="26" t="inlineStr">
+      <c r="A184" s="28" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B184" s="27" t="n"/>
-      <c r="C184" s="28" t="inlineStr">
+      <c r="B184" s="29" t="n"/>
+      <c r="C184" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 38 points 1-4
 </t>
         </is>
       </c>
-      <c r="D184" s="29" t="n">
+      <c r="D184" s="31" t="n">
         <v>0.3590277777777778</v>
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="26" t="inlineStr">
+      <c r="A185" s="28" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B185" s="27" t="n"/>
-      <c r="C185" s="28" t="inlineStr">
+      <c r="B185" s="29" t="n"/>
+      <c r="C185" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
  </t>
         </is>
       </c>
-      <c r="D185" s="29" t="n">
+      <c r="D185" s="31" t="n">
         <v>0.3611111111111111</v>
       </c>
     </row>
@@ -3175,21 +3190,21 @@
       <c r="A186" s="15" t="n"/>
       <c r="B186" s="15" t="n"/>
       <c r="C186" s="15" t="inlineStr"/>
-      <c r="D186" s="25" t="n"/>
+      <c r="D186" s="27" t="n"/>
     </row>
     <row r="187">
-      <c r="A187" s="39" t="inlineStr">
+      <c r="A187" s="43" t="inlineStr">
         <is>
           <t>Song 141</t>
         </is>
       </c>
-      <c r="B187" s="27" t="n"/>
-      <c r="C187" s="40" t="inlineStr">
+      <c r="B187" s="29" t="n"/>
+      <c r="C187" s="44" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D187" s="36" t="n"/>
+      <c r="D187" s="38" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Cleaned up code and directory structure
</commit_message>
<xml_diff>
--- a/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
+++ b/output/Life and Ministry Meeting Workbook, January-February 2023.xlsx
@@ -102,7 +102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00282a36"/>
+        <fgColor rgb="0093684c"/>
       </patternFill>
     </fill>
     <fill>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -325,20 +325,14 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,7 +814,7 @@
       </c>
       <c r="B6" s="27" t="inlineStr">
         <is>
-          <t>Abigail Corran</t>
+          <t>Ben Corran</t>
         </is>
       </c>
       <c r="C6" s="28" t="inlineStr">
@@ -841,7 +835,7 @@
       </c>
       <c r="B7" s="27" t="inlineStr">
         <is>
-          <t>Ron Crowly</t>
+          <t>Graham Haynes</t>
         </is>
       </c>
       <c r="C7" s="28" t="inlineStr">
@@ -940,11 +934,7 @@
     </row>
     <row r="14">
       <c r="A14" s="30" t="n"/>
-      <c r="B14" s="36" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
+      <c r="B14" s="36" t="n"/>
       <c r="C14" s="30" t="n"/>
       <c r="D14" s="37" t="n"/>
     </row>
@@ -954,12 +944,8 @@
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B15" s="38" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="C15" s="39" t="inlineStr">
+      <c r="B15" s="15" t="n"/>
+      <c r="C15" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 16)
 </t>
@@ -971,11 +957,7 @@
     </row>
     <row r="16">
       <c r="A16" s="30" t="n"/>
-      <c r="B16" s="36" t="inlineStr">
-        <is>
-          <t>basdf</t>
-        </is>
-      </c>
+      <c r="B16" s="36" t="n"/>
       <c r="C16" s="30" t="n"/>
       <c r="D16" s="37" t="n"/>
     </row>
@@ -992,7 +974,7 @@
         </is>
       </c>
       <c r="B18" s="15" t="n"/>
-      <c r="C18" s="40" t="inlineStr">
+      <c r="C18" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -1235,11 +1217,7 @@
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B35" s="38" t="inlineStr">
-        <is>
-          <t>dddd</t>
-        </is>
-      </c>
+      <c r="B35" s="15" t="n"/>
       <c r="C35" s="34" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Use the sample conversation topic. (th study 15)
@@ -1252,11 +1230,7 @@
     </row>
     <row r="36">
       <c r="A36" s="30" t="n"/>
-      <c r="B36" s="36" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
+      <c r="B36" s="36" t="n"/>
       <c r="C36" s="30" t="n"/>
       <c r="D36" s="37" t="n"/>
     </row>
@@ -1267,7 +1241,7 @@
         </is>
       </c>
       <c r="B37" s="15" t="n"/>
-      <c r="C37" s="39" t="inlineStr">
+      <c r="C37" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 19)
 </t>
@@ -1279,11 +1253,7 @@
     </row>
     <row r="38">
       <c r="A38" s="30" t="n"/>
-      <c r="B38" s="36" t="inlineStr">
-        <is>
-          <t>David Moore</t>
-        </is>
-      </c>
+      <c r="B38" s="36" t="n"/>
       <c r="C38" s="30" t="n"/>
       <c r="D38" s="37" t="n"/>
     </row>
@@ -1300,7 +1270,7 @@
         </is>
       </c>
       <c r="B40" s="15" t="n"/>
-      <c r="C40" s="40" t="inlineStr">
+      <c r="C40" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -1527,7 +1497,7 @@
         </is>
       </c>
       <c r="B56" s="15" t="n"/>
-      <c r="C56" s="39" t="inlineStr">
+      <c r="C56" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a magazine to address a topic raised by the householder. (th study 4)
 </t>
@@ -1539,7 +1509,7 @@
     </row>
     <row r="57">
       <c r="A57" s="30" t="n"/>
-      <c r="B57" s="41" t="n"/>
+      <c r="B57" s="36" t="n"/>
       <c r="C57" s="30" t="n"/>
       <c r="D57" s="37" t="n"/>
     </row>
@@ -1550,7 +1520,7 @@
         </is>
       </c>
       <c r="B58" s="15" t="n"/>
-      <c r="C58" s="39" t="inlineStr">
+      <c r="C58" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 1)
 </t>
@@ -1562,7 +1532,7 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="30" t="n"/>
-      <c r="B59" s="41" t="n"/>
+      <c r="B59" s="36" t="n"/>
       <c r="C59" s="30" t="n"/>
       <c r="D59" s="37" t="n"/>
     </row>
@@ -1573,7 +1543,7 @@
         </is>
       </c>
       <c r="B60" s="15" t="n"/>
-      <c r="C60" s="39" t="inlineStr">
+      <c r="C60" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 point 7 and Some People Say (th study 8)
 </t>
@@ -1585,7 +1555,7 @@
     </row>
     <row r="61">
       <c r="A61" s="30" t="n"/>
-      <c r="B61" s="41" t="n"/>
+      <c r="B61" s="36" t="n"/>
       <c r="C61" s="30" t="n"/>
       <c r="D61" s="37" t="n"/>
     </row>
@@ -1602,7 +1572,7 @@
         </is>
       </c>
       <c r="B63" s="15" t="n"/>
-      <c r="C63" s="40" t="inlineStr">
+      <c r="C63" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -1829,7 +1799,7 @@
         </is>
       </c>
       <c r="B79" s="15" t="n"/>
-      <c r="C79" s="39" t="inlineStr">
+      <c r="C79" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Use the sample conversation topic. Respond to a common objection. (th study 3)
 </t>
@@ -1841,7 +1811,7 @@
     </row>
     <row r="80">
       <c r="A80" s="30" t="n"/>
-      <c r="B80" s="41" t="n"/>
+      <c r="B80" s="36" t="n"/>
       <c r="C80" s="30" t="n"/>
       <c r="D80" s="37" t="n"/>
     </row>
@@ -1852,7 +1822,7 @@
         </is>
       </c>
       <c r="B81" s="15" t="n"/>
-      <c r="C81" s="39" t="inlineStr">
+      <c r="C81" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Why Study the Bible? (th study 14)
 </t>
@@ -1864,7 +1834,7 @@
     </row>
     <row r="82">
       <c r="A82" s="30" t="n"/>
-      <c r="B82" s="41" t="n"/>
+      <c r="B82" s="36" t="n"/>
       <c r="C82" s="30" t="n"/>
       <c r="D82" s="37" t="n"/>
     </row>
@@ -1875,7 +1845,7 @@
         </is>
       </c>
       <c r="B83" s="15" t="n"/>
-      <c r="C83" s="39" t="inlineStr">
+      <c r="C83" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 summary, review, and goal (th study 9)
 </t>
@@ -1887,7 +1857,7 @@
     </row>
     <row r="84">
       <c r="A84" s="30" t="n"/>
-      <c r="B84" s="41" t="n"/>
+      <c r="B84" s="36" t="n"/>
       <c r="C84" s="30" t="n"/>
       <c r="D84" s="37" t="n"/>
     </row>
@@ -1904,7 +1874,7 @@
         </is>
       </c>
       <c r="B86" s="15" t="n"/>
-      <c r="C86" s="40" t="inlineStr">
+      <c r="C86" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -1963,13 +1933,13 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="42" t="inlineStr">
+      <c r="A90" s="40" t="inlineStr">
         <is>
           <t>Song 88</t>
         </is>
       </c>
       <c r="B90" s="30" t="n"/>
-      <c r="C90" s="43" t="inlineStr">
+      <c r="C90" s="41" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
@@ -1979,23 +1949,23 @@
     <row r="91">
       <c r="A91" s="15" t="n"/>
       <c r="B91" s="15" t="n"/>
-      <c r="C91" s="44" t="n"/>
+      <c r="C91" s="42" t="n"/>
       <c r="D91" s="15" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="15" t="n"/>
       <c r="B92" s="15" t="n"/>
-      <c r="C92" s="44" t="n"/>
+      <c r="C92" s="42" t="n"/>
       <c r="D92" s="15" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="15" t="n"/>
-      <c r="B93" s="45" t="inlineStr">
+      <c r="B93" s="43" t="inlineStr">
         <is>
           <t>Life and Ministry Meeting Workbook, February 2023</t>
         </is>
       </c>
-      <c r="C93" s="46" t="n"/>
+      <c r="C93" s="44" t="n"/>
       <c r="D93" s="15" t="n"/>
     </row>
     <row r="94">
@@ -2004,7 +1974,7 @@
           <t>Week 1</t>
         </is>
       </c>
-      <c r="B94" s="47" t="inlineStr">
+      <c r="B94" s="45" t="inlineStr">
         <is>
           <t>January 30 - February 5</t>
         </is>
@@ -2147,7 +2117,7 @@
         </is>
       </c>
       <c r="B104" s="15" t="n"/>
-      <c r="C104" s="39" t="inlineStr">
+      <c r="C104" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Leave a jw.org contact card. (th study 16)
 </t>
@@ -2159,7 +2129,7 @@
     </row>
     <row r="105">
       <c r="A105" s="30" t="n"/>
-      <c r="B105" s="41" t="n"/>
+      <c r="B105" s="36" t="n"/>
       <c r="C105" s="30" t="n"/>
       <c r="D105" s="37" t="n"/>
     </row>
@@ -2170,7 +2140,7 @@
         </is>
       </c>
       <c r="B106" s="15" t="n"/>
-      <c r="C106" s="39" t="inlineStr">
+      <c r="C106" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 20)
 </t>
@@ -2182,7 +2152,7 @@
     </row>
     <row r="107">
       <c r="A107" s="30" t="n"/>
-      <c r="B107" s="41" t="n"/>
+      <c r="B107" s="36" t="n"/>
       <c r="C107" s="30" t="n"/>
       <c r="D107" s="37" t="n"/>
     </row>
@@ -2193,7 +2163,7 @@
         </is>
       </c>
       <c r="B108" s="15" t="n"/>
-      <c r="C108" s="39" t="inlineStr">
+      <c r="C108" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w21.06 3-4 ¶3-8 —Theme: Help Your Bible Student to Apply What He Is Learning. (th study 13)
 </t>
@@ -2205,7 +2175,7 @@
     </row>
     <row r="109">
       <c r="A109" s="30" t="n"/>
-      <c r="B109" s="41" t="n"/>
+      <c r="B109" s="36" t="n"/>
       <c r="C109" s="30" t="n"/>
       <c r="D109" s="37" t="n"/>
     </row>
@@ -2222,7 +2192,7 @@
         </is>
       </c>
       <c r="B111" s="15" t="n"/>
-      <c r="C111" s="40" t="inlineStr">
+      <c r="C111" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -2449,7 +2419,7 @@
         </is>
       </c>
       <c r="B127" s="15" t="n"/>
-      <c r="C127" s="39" t="inlineStr">
+      <c r="C127" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a Bible study. (th study 12)
 </t>
@@ -2461,7 +2431,7 @@
     </row>
     <row r="128">
       <c r="A128" s="30" t="n"/>
-      <c r="B128" s="41" t="n"/>
+      <c r="B128" s="36" t="n"/>
       <c r="C128" s="30" t="n"/>
       <c r="D128" s="37" t="n"/>
     </row>
@@ -2472,7 +2442,7 @@
         </is>
       </c>
       <c r="B129" s="15" t="n"/>
-      <c r="C129" s="39" t="inlineStr">
+      <c r="C129" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video What Happens at a Bible Study? (th study 6)
 </t>
@@ -2484,7 +2454,7 @@
     </row>
     <row r="130">
       <c r="A130" s="30" t="n"/>
-      <c r="B130" s="41" t="n"/>
+      <c r="B130" s="36" t="n"/>
       <c r="C130" s="30" t="n"/>
       <c r="D130" s="37" t="n"/>
     </row>
@@ -2507,7 +2477,7 @@
     </row>
     <row r="132">
       <c r="A132" s="30" t="n"/>
-      <c r="B132" s="41" t="n"/>
+      <c r="B132" s="36" t="n"/>
       <c r="C132" s="30" t="n"/>
       <c r="D132" s="37" t="n"/>
     </row>
@@ -2524,7 +2494,7 @@
         </is>
       </c>
       <c r="B134" s="15" t="n"/>
-      <c r="C134" s="40" t="inlineStr">
+      <c r="C134" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -2768,7 +2738,7 @@
         </is>
       </c>
       <c r="B151" s="15" t="n"/>
-      <c r="C151" s="39" t="inlineStr">
+      <c r="C151" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Respond to a common objection. (th study 18)
 </t>
@@ -2780,7 +2750,7 @@
     </row>
     <row r="152">
       <c r="A152" s="30" t="n"/>
-      <c r="B152" s="41" t="n"/>
+      <c r="B152" s="36" t="n"/>
       <c r="C152" s="30" t="n"/>
       <c r="D152" s="37" t="n"/>
     </row>
@@ -2791,7 +2761,7 @@
         </is>
       </c>
       <c r="B153" s="15" t="n"/>
-      <c r="C153" s="39" t="inlineStr">
+      <c r="C153" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 7)
 </t>
@@ -2803,7 +2773,7 @@
     </row>
     <row r="154">
       <c r="A154" s="30" t="n"/>
-      <c r="B154" s="41" t="n"/>
+      <c r="B154" s="36" t="n"/>
       <c r="C154" s="30" t="n"/>
       <c r="D154" s="37" t="n"/>
     </row>
@@ -2814,7 +2784,7 @@
         </is>
       </c>
       <c r="B155" s="15" t="n"/>
-      <c r="C155" s="39" t="inlineStr">
+      <c r="C155" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w16.01 13-14 ¶7-10 —Theme: “The Love the Christ Has Compels Us.” —2Co 5:14. (th study 8)
 </t>
@@ -2826,7 +2796,7 @@
     </row>
     <row r="156">
       <c r="A156" s="30" t="n"/>
-      <c r="B156" s="41" t="n"/>
+      <c r="B156" s="36" t="n"/>
       <c r="C156" s="30" t="n"/>
       <c r="D156" s="37" t="n"/>
     </row>
@@ -2843,7 +2813,7 @@
         </is>
       </c>
       <c r="B158" s="15" t="n"/>
-      <c r="C158" s="40" t="inlineStr">
+      <c r="C158" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -3087,7 +3057,7 @@
         </is>
       </c>
       <c r="B175" s="15" t="n"/>
-      <c r="C175" s="39" t="inlineStr">
+      <c r="C175" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Jehovah’s Witnesses —Who Are We? (th study 17)
 </t>
@@ -3099,7 +3069,7 @@
     </row>
     <row r="176">
       <c r="A176" s="30" t="n"/>
-      <c r="B176" s="41" t="n"/>
+      <c r="B176" s="36" t="n"/>
       <c r="C176" s="30" t="n"/>
       <c r="D176" s="37" t="n"/>
     </row>
@@ -3110,7 +3080,7 @@
         </is>
       </c>
       <c r="B177" s="15" t="n"/>
-      <c r="C177" s="39" t="inlineStr">
+      <c r="C177" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 3)
 </t>
@@ -3122,7 +3092,7 @@
     </row>
     <row r="178">
       <c r="A178" s="30" t="n"/>
-      <c r="B178" s="41" t="n"/>
+      <c r="B178" s="36" t="n"/>
       <c r="C178" s="30" t="n"/>
       <c r="D178" s="37" t="n"/>
     </row>
@@ -3145,7 +3115,7 @@
     </row>
     <row r="180">
       <c r="A180" s="30" t="n"/>
-      <c r="B180" s="41" t="n"/>
+      <c r="B180" s="36" t="n"/>
       <c r="C180" s="30" t="n"/>
       <c r="D180" s="37" t="n"/>
     </row>
@@ -3162,7 +3132,7 @@
         </is>
       </c>
       <c r="B182" s="15" t="n"/>
-      <c r="C182" s="40" t="inlineStr">
+      <c r="C182" s="39" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
@@ -3227,13 +3197,13 @@
       <c r="D186" s="25" t="n"/>
     </row>
     <row r="187">
-      <c r="A187" s="42" t="inlineStr">
+      <c r="A187" s="40" t="inlineStr">
         <is>
           <t>Song 141</t>
         </is>
       </c>
       <c r="B187" s="30" t="n"/>
-      <c r="C187" s="43" t="inlineStr">
+      <c r="C187" s="41" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>

</xml_diff>